<commit_message>
read excel files with openpyxl
</commit_message>
<xml_diff>
--- a/latamReturns&Ratios/latamCountriesRatios.xlsx
+++ b/latamReturns&Ratios/latamCountriesRatios.xlsx
@@ -29,7 +29,7 @@
       <b val="1"/>
     </font>
   </fonts>
-  <fills count="37">
+  <fills count="33">
     <fill>
       <patternFill/>
     </fill>
@@ -38,177 +38,157 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00F4B60D"/>
+        <fgColor rgb="00FC8C9D"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="009D05B2"/>
+        <fgColor rgb="00452633"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="0054CB5E"/>
+        <fgColor rgb="008DE2B9"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="0053CE7F"/>
+        <fgColor rgb="00D721FC"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="003DBF54"/>
+        <fgColor rgb="00CD504B"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="0096FAD9"/>
+        <fgColor rgb="00943BFA"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00E92EFA"/>
+        <fgColor rgb="00D05947"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00780FD7"/>
+        <fgColor rgb="004F9B3A"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00576620"/>
+        <fgColor rgb="006481CE"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="001D2D81"/>
+        <fgColor rgb="00D05614"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00F5F269"/>
+        <fgColor rgb="00806892"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="0013DE1C"/>
+        <fgColor rgb="00E7B6C3"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="000B40CC"/>
+        <fgColor rgb="00CD7D02"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="0085843D"/>
+        <fgColor rgb="0081460E"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="008843CE"/>
+        <fgColor rgb="00DA2D12"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00F9EE35"/>
+        <fgColor rgb="00C09744"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00646E5C"/>
+        <fgColor rgb="00F1F705"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="0078543A"/>
+        <fgColor rgb="0075EA01"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00CABBDF"/>
+        <fgColor rgb="00C4BEBE"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00F53DB9"/>
+        <fgColor rgb="00874A3E"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00685F08"/>
+        <fgColor rgb="00D5D3C6"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="008EAF52"/>
+        <fgColor rgb="00FB6DC3"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00DECAEC"/>
+        <fgColor rgb="00BC6D11"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00CCC146"/>
+        <fgColor rgb="0016232A"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00722EB6"/>
+        <fgColor rgb="00BABAE5"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="008D9208"/>
+        <fgColor rgb="00B75069"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00CAFBAA"/>
+        <fgColor rgb="0060368C"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="0049E819"/>
+        <fgColor rgb="0001F2F9"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="0051D6E8"/>
+        <fgColor rgb="002E8337"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="0047E42C"/>
+        <fgColor rgb="0086D738"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00D26336"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="00BA9C6A"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="007D72AC"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="0065FFBF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="00AB395A"/>
+        <fgColor rgb="005AD4D9"/>
       </patternFill>
     </fill>
   </fills>
@@ -230,7 +210,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
@@ -266,10 +246,6 @@
     <xf numFmtId="0" fontId="0" fillId="30" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="31" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="32" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="36" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -635,7 +611,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C254"/>
+  <dimension ref="A1:C235"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -667,7 +643,7 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>2.3</v>
+        <v>2.03</v>
       </c>
     </row>
     <row r="3">
@@ -682,7 +658,7 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>2.05</v>
+        <v>2.12</v>
       </c>
     </row>
     <row r="4">
@@ -697,7 +673,7 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>2.12</v>
+        <v>2.09</v>
       </c>
     </row>
     <row r="5">
@@ -712,7 +688,7 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>2.39</v>
+        <v>2.63</v>
       </c>
     </row>
     <row r="6">
@@ -727,7 +703,7 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>2.41</v>
+        <v>2.34</v>
       </c>
     </row>
     <row r="7">
@@ -742,7 +718,7 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>2.12</v>
+        <v>2.45</v>
       </c>
     </row>
     <row r="8">
@@ -757,7 +733,7 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>2</v>
+        <v>2.26</v>
       </c>
     </row>
     <row r="9">
@@ -772,7 +748,7 @@
         </is>
       </c>
       <c r="C9" t="n">
-        <v>2.23</v>
+        <v>2.38</v>
       </c>
     </row>
     <row r="10">
@@ -787,7 +763,7 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>2.29</v>
+        <v>2.15</v>
       </c>
     </row>
     <row r="11">
@@ -802,7 +778,7 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>2.75</v>
+        <v>3.27</v>
       </c>
     </row>
     <row r="12">
@@ -817,13 +793,13 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>2.54</v>
+        <v>2.47</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="inlineStr">
         <is>
-          <t>GGAL/TGS</t>
+          <t>GGAL/CRESY</t>
         </is>
       </c>
       <c r="B13" s="4" t="inlineStr">
@@ -832,13 +808,13 @@
         </is>
       </c>
       <c r="C13" t="n">
-        <v>2.02</v>
+        <v>2.17</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="inlineStr">
         <is>
-          <t>GGAL/BBAR</t>
+          <t>GGAL/TGS</t>
         </is>
       </c>
       <c r="B14" s="4" t="inlineStr">
@@ -847,13 +823,13 @@
         </is>
       </c>
       <c r="C14" t="n">
-        <v>2.31</v>
+        <v>2.27</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="inlineStr">
         <is>
-          <t>GGAL/LOMA</t>
+          <t>GGAL/BBAR</t>
         </is>
       </c>
       <c r="B15" s="4" t="inlineStr">
@@ -862,13 +838,13 @@
         </is>
       </c>
       <c r="C15" t="n">
-        <v>2.27</v>
+        <v>2.31</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="inlineStr">
         <is>
-          <t>GGAL/IRS</t>
+          <t>GGAL/LOMA</t>
         </is>
       </c>
       <c r="B16" s="4" t="inlineStr">
@@ -877,13 +853,13 @@
         </is>
       </c>
       <c r="C16" t="n">
-        <v>2.39</v>
+        <v>2.44</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="inlineStr">
         <is>
-          <t>GGAL/PAM</t>
+          <t>GGAL/IRS</t>
         </is>
       </c>
       <c r="B17" s="4" t="inlineStr">
@@ -892,28 +868,28 @@
         </is>
       </c>
       <c r="C17" t="n">
-        <v>2.79</v>
+        <v>2.27</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="inlineStr">
         <is>
-          <t>SUPV/AGRO</t>
-        </is>
-      </c>
-      <c r="B18" s="5" t="inlineStr">
-        <is>
-          <t>SUPV</t>
+          <t>GGAL/PAM</t>
+        </is>
+      </c>
+      <c r="B18" s="4" t="inlineStr">
+        <is>
+          <t>GGAL</t>
         </is>
       </c>
       <c r="C18" t="n">
-        <v>2.06</v>
+        <v>3.31</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="inlineStr">
         <is>
-          <t>SUPV/TGS</t>
+          <t>SUPV/AGRO</t>
         </is>
       </c>
       <c r="B19" s="5" t="inlineStr">
@@ -922,13 +898,13 @@
         </is>
       </c>
       <c r="C19" t="n">
-        <v>2</v>
+        <v>2.15</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="inlineStr">
         <is>
-          <t>SUPV/LOMA</t>
+          <t>SUPV/CRESY</t>
         </is>
       </c>
       <c r="B20" s="5" t="inlineStr">
@@ -937,13 +913,13 @@
         </is>
       </c>
       <c r="C20" t="n">
-        <v>2.14</v>
+        <v>2.37</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="inlineStr">
         <is>
-          <t>SUPV/PAM</t>
+          <t>SUPV/TGS</t>
         </is>
       </c>
       <c r="B21" s="5" t="inlineStr">
@@ -952,148 +928,148 @@
         </is>
       </c>
       <c r="C21" t="n">
-        <v>2.21</v>
+        <v>2.38</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="1" t="inlineStr">
         <is>
-          <t>PAM/TEO</t>
-        </is>
-      </c>
-      <c r="B22" s="6" t="inlineStr">
-        <is>
-          <t>PAM</t>
+          <t>SUPV/LOMA</t>
+        </is>
+      </c>
+      <c r="B22" s="5" t="inlineStr">
+        <is>
+          <t>SUPV</t>
         </is>
       </c>
       <c r="C22" t="n">
-        <v>-2.02</v>
+        <v>2.42</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="1" t="inlineStr">
         <is>
-          <t>PAM/YPF</t>
-        </is>
-      </c>
-      <c r="B23" s="6" t="inlineStr">
-        <is>
-          <t>PAM</t>
+          <t>SUPV/IRS</t>
+        </is>
+      </c>
+      <c r="B23" s="5" t="inlineStr">
+        <is>
+          <t>SUPV</t>
         </is>
       </c>
       <c r="C23" t="n">
-        <v>-2.04</v>
+        <v>2.03</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="1" t="inlineStr">
         <is>
-          <t>PAM/BMA</t>
-        </is>
-      </c>
-      <c r="B24" s="6" t="inlineStr">
-        <is>
-          <t>PAM</t>
+          <t>SUPV/CEPU</t>
+        </is>
+      </c>
+      <c r="B24" s="5" t="inlineStr">
+        <is>
+          <t>SUPV</t>
         </is>
       </c>
       <c r="C24" t="n">
-        <v>-2.23</v>
+        <v>2.05</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="1" t="inlineStr">
         <is>
-          <t>PAM/GGAL</t>
-        </is>
-      </c>
-      <c r="B25" s="6" t="inlineStr">
-        <is>
-          <t>PAM</t>
+          <t>SUPV/PAM</t>
+        </is>
+      </c>
+      <c r="B25" s="5" t="inlineStr">
+        <is>
+          <t>SUPV</t>
         </is>
       </c>
       <c r="C25" t="n">
-        <v>-2.24</v>
+        <v>2.75</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="1" t="inlineStr">
         <is>
-          <t>VIV/ABEV</t>
-        </is>
-      </c>
-      <c r="B26" s="7" t="inlineStr">
-        <is>
-          <t>VIV</t>
+          <t>PAM/TEO</t>
+        </is>
+      </c>
+      <c r="B26" s="6" t="inlineStr">
+        <is>
+          <t>PAM</t>
         </is>
       </c>
       <c r="C26" t="n">
-        <v>2.13</v>
+        <v>-2.18</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="1" t="inlineStr">
         <is>
-          <t>VIV/BBD</t>
-        </is>
-      </c>
-      <c r="B27" s="7" t="inlineStr">
-        <is>
-          <t>VIV</t>
+          <t>PAM/YPF</t>
+        </is>
+      </c>
+      <c r="B27" s="6" t="inlineStr">
+        <is>
+          <t>PAM</t>
         </is>
       </c>
       <c r="C27" t="n">
-        <v>3.44</v>
+        <v>-2.27</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="1" t="inlineStr">
         <is>
-          <t>VIV/BSBR</t>
-        </is>
-      </c>
-      <c r="B28" s="7" t="inlineStr">
-        <is>
-          <t>VIV</t>
+          <t>PAM/VIST</t>
+        </is>
+      </c>
+      <c r="B28" s="6" t="inlineStr">
+        <is>
+          <t>PAM</t>
         </is>
       </c>
       <c r="C28" t="n">
-        <v>2.41</v>
+        <v>-2.18</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="1" t="inlineStr">
         <is>
-          <t>VIV/GOL</t>
-        </is>
-      </c>
-      <c r="B29" s="7" t="inlineStr">
-        <is>
-          <t>VIV</t>
+          <t>PAM/BMA</t>
+        </is>
+      </c>
+      <c r="B29" s="6" t="inlineStr">
+        <is>
+          <t>PAM</t>
         </is>
       </c>
       <c r="C29" t="n">
-        <v>4.23</v>
+        <v>-2.54</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="1" t="inlineStr">
         <is>
-          <t>VIV/GGB</t>
-        </is>
-      </c>
-      <c r="B30" s="7" t="inlineStr">
-        <is>
-          <t>VIV</t>
+          <t>PAM/GGAL</t>
+        </is>
+      </c>
+      <c r="B30" s="6" t="inlineStr">
+        <is>
+          <t>PAM</t>
         </is>
       </c>
       <c r="C30" t="n">
-        <v>2.25</v>
+        <v>-2.54</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="1" t="inlineStr">
         <is>
-          <t>VIV/VALE</t>
+          <t>VIV/ABEV</t>
         </is>
       </c>
       <c r="B31" s="7" t="inlineStr">
@@ -1102,13 +1078,13 @@
         </is>
       </c>
       <c r="C31" t="n">
-        <v>2.21</v>
+        <v>2.01</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="1" t="inlineStr">
         <is>
-          <t>VIV/SGML</t>
+          <t>VIV/BBD</t>
         </is>
       </c>
       <c r="B32" s="7" t="inlineStr">
@@ -1117,13 +1093,13 @@
         </is>
       </c>
       <c r="C32" t="n">
-        <v>3.87</v>
+        <v>3.05</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="1" t="inlineStr">
         <is>
-          <t>VIV/ELP</t>
+          <t>VIV/GOL</t>
         </is>
       </c>
       <c r="B33" s="7" t="inlineStr">
@@ -1132,58 +1108,58 @@
         </is>
       </c>
       <c r="C33" t="n">
-        <v>2.43</v>
+        <v>4.22</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="1" t="inlineStr">
         <is>
-          <t>TIMB/ABEV</t>
-        </is>
-      </c>
-      <c r="B34" s="8" t="inlineStr">
-        <is>
-          <t>TIMB</t>
+          <t>VIV/SGML</t>
+        </is>
+      </c>
+      <c r="B34" s="7" t="inlineStr">
+        <is>
+          <t>VIV</t>
         </is>
       </c>
       <c r="C34" t="n">
-        <v>2.01</v>
+        <v>3.5</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="1" t="inlineStr">
         <is>
-          <t>TIMB/BBD</t>
-        </is>
-      </c>
-      <c r="B35" s="8" t="inlineStr">
-        <is>
-          <t>TIMB</t>
+          <t>VIV/ELP</t>
+        </is>
+      </c>
+      <c r="B35" s="7" t="inlineStr">
+        <is>
+          <t>VIV</t>
         </is>
       </c>
       <c r="C35" t="n">
-        <v>3.28</v>
+        <v>2.09</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="1" t="inlineStr">
         <is>
-          <t>TIMB/BSBR</t>
-        </is>
-      </c>
-      <c r="B36" s="8" t="inlineStr">
-        <is>
-          <t>TIMB</t>
+          <t>VIV/SBS</t>
+        </is>
+      </c>
+      <c r="B36" s="7" t="inlineStr">
+        <is>
+          <t>VIV</t>
         </is>
       </c>
       <c r="C36" t="n">
-        <v>2.14</v>
+        <v>-2.15</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="1" t="inlineStr">
         <is>
-          <t>TIMB/AZUL</t>
+          <t>TIMB/UGP</t>
         </is>
       </c>
       <c r="B37" s="8" t="inlineStr">
@@ -1192,13 +1168,13 @@
         </is>
       </c>
       <c r="C37" t="n">
-        <v>2</v>
+        <v>-2.03</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="1" t="inlineStr">
         <is>
-          <t>TIMB/GOL</t>
+          <t>TIMB/BBD</t>
         </is>
       </c>
       <c r="B38" s="8" t="inlineStr">
@@ -1207,13 +1183,13 @@
         </is>
       </c>
       <c r="C38" t="n">
-        <v>4.14</v>
+        <v>2.76</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="1" t="inlineStr">
         <is>
-          <t>TIMB/GGB</t>
+          <t>TIMB/GOL</t>
         </is>
       </c>
       <c r="B39" s="8" t="inlineStr">
@@ -1222,7 +1198,7 @@
         </is>
       </c>
       <c r="C39" t="n">
-        <v>2.15</v>
+        <v>4.07</v>
       </c>
     </row>
     <row r="40">
@@ -1237,13 +1213,13 @@
         </is>
       </c>
       <c r="C40" t="n">
-        <v>3.76</v>
+        <v>3.34</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="1" t="inlineStr">
         <is>
-          <t>TIMB/ELP</t>
+          <t>TIMB/SBS</t>
         </is>
       </c>
       <c r="B41" s="8" t="inlineStr">
@@ -1252,7 +1228,7 @@
         </is>
       </c>
       <c r="C41" t="n">
-        <v>2.39</v>
+        <v>-2.38</v>
       </c>
     </row>
     <row r="42">
@@ -1267,7 +1243,7 @@
         </is>
       </c>
       <c r="C42" t="n">
-        <v>-2.01</v>
+        <v>-2.14</v>
       </c>
     </row>
     <row r="43">
@@ -1282,13 +1258,13 @@
         </is>
       </c>
       <c r="C43" t="n">
-        <v>-2.2</v>
+        <v>-2.09</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="1" t="inlineStr">
         <is>
-          <t>ABEV/GOL</t>
+          <t>ABEV/ERJ</t>
         </is>
       </c>
       <c r="B44" s="9" t="inlineStr">
@@ -1297,13 +1273,13 @@
         </is>
       </c>
       <c r="C44" t="n">
-        <v>3.89</v>
+        <v>-2</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="1" t="inlineStr">
         <is>
-          <t>ABEV/SGML</t>
+          <t>ABEV/GOL</t>
         </is>
       </c>
       <c r="B45" s="9" t="inlineStr">
@@ -1312,13 +1288,13 @@
         </is>
       </c>
       <c r="C45" t="n">
-        <v>4.03</v>
+        <v>4</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="1" t="inlineStr">
         <is>
-          <t>ABEV/EBR</t>
+          <t>ABEV/SID</t>
         </is>
       </c>
       <c r="B46" s="9" t="inlineStr">
@@ -1327,43 +1303,43 @@
         </is>
       </c>
       <c r="C46" t="n">
-        <v>-2.1</v>
+        <v>-2.03</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="1" t="inlineStr">
         <is>
-          <t>BRFS/BBD</t>
-        </is>
-      </c>
-      <c r="B47" s="10" t="inlineStr">
-        <is>
-          <t>BRFS</t>
+          <t>ABEV/SGML</t>
+        </is>
+      </c>
+      <c r="B47" s="9" t="inlineStr">
+        <is>
+          <t>ABEV</t>
         </is>
       </c>
       <c r="C47" t="n">
-        <v>2.49</v>
+        <v>3.67</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="1" t="inlineStr">
         <is>
-          <t>BRFS/AZUL</t>
-        </is>
-      </c>
-      <c r="B48" s="10" t="inlineStr">
-        <is>
-          <t>BRFS</t>
+          <t>ABEV/EBR</t>
+        </is>
+      </c>
+      <c r="B48" s="9" t="inlineStr">
+        <is>
+          <t>ABEV</t>
         </is>
       </c>
       <c r="C48" t="n">
-        <v>2.46</v>
+        <v>-2.09</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" s="1" t="inlineStr">
         <is>
-          <t>BRFS/GOL</t>
+          <t>BRFS/BBD</t>
         </is>
       </c>
       <c r="B49" s="10" t="inlineStr">
@@ -1372,13 +1348,13 @@
         </is>
       </c>
       <c r="C49" t="n">
-        <v>4.02</v>
+        <v>2.46</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" s="1" t="inlineStr">
         <is>
-          <t>BRFS/SGML</t>
+          <t>BRFS/AZUL</t>
         </is>
       </c>
       <c r="B50" s="10" t="inlineStr">
@@ -1387,13 +1363,13 @@
         </is>
       </c>
       <c r="C50" t="n">
-        <v>3.48</v>
+        <v>2.49</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" s="1" t="inlineStr">
         <is>
-          <t>BRFS/ELP</t>
+          <t>BRFS/GOL</t>
         </is>
       </c>
       <c r="B51" s="10" t="inlineStr">
@@ -1402,43 +1378,43 @@
         </is>
       </c>
       <c r="C51" t="n">
-        <v>2.03</v>
+        <v>4.16</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" s="1" t="inlineStr">
         <is>
-          <t>PBR/ABEV</t>
-        </is>
-      </c>
-      <c r="B52" s="11" t="inlineStr">
-        <is>
-          <t>PBR</t>
+          <t>BRFS/SGML</t>
+        </is>
+      </c>
+      <c r="B52" s="10" t="inlineStr">
+        <is>
+          <t>BRFS</t>
         </is>
       </c>
       <c r="C52" t="n">
-        <v>2.03</v>
+        <v>3.32</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" s="1" t="inlineStr">
         <is>
-          <t>PBR/BBD</t>
-        </is>
-      </c>
-      <c r="B53" s="11" t="inlineStr">
-        <is>
-          <t>PBR</t>
+          <t>BRFS/ELP</t>
+        </is>
+      </c>
+      <c r="B53" s="10" t="inlineStr">
+        <is>
+          <t>BRFS</t>
         </is>
       </c>
       <c r="C53" t="n">
-        <v>3.01</v>
+        <v>2.04</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" s="1" t="inlineStr">
         <is>
-          <t>PBR/AZUL</t>
+          <t>PBR/ABEV</t>
         </is>
       </c>
       <c r="B54" s="11" t="inlineStr">
@@ -1447,13 +1423,13 @@
         </is>
       </c>
       <c r="C54" t="n">
-        <v>2.2</v>
+        <v>2.22</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" s="1" t="inlineStr">
         <is>
-          <t>PBR/GOL</t>
+          <t>PBR/BBD</t>
         </is>
       </c>
       <c r="B55" s="11" t="inlineStr">
@@ -1462,13 +1438,13 @@
         </is>
       </c>
       <c r="C55" t="n">
-        <v>4.19</v>
+        <v>3.09</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" s="1" t="inlineStr">
         <is>
-          <t>PBR/GGB</t>
+          <t>PBR/AZUL</t>
         </is>
       </c>
       <c r="B56" s="11" t="inlineStr">
@@ -1477,13 +1453,13 @@
         </is>
       </c>
       <c r="C56" t="n">
-        <v>2.33</v>
+        <v>2.39</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" s="1" t="inlineStr">
         <is>
-          <t>PBR/SUZ</t>
+          <t>PBR/GOL</t>
         </is>
       </c>
       <c r="B57" s="11" t="inlineStr">
@@ -1492,13 +1468,13 @@
         </is>
       </c>
       <c r="C57" t="n">
-        <v>2.5</v>
+        <v>4.41</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" s="1" t="inlineStr">
         <is>
-          <t>PBR/BAK</t>
+          <t>PBR/GGB</t>
         </is>
       </c>
       <c r="B58" s="11" t="inlineStr">
@@ -1507,13 +1483,13 @@
         </is>
       </c>
       <c r="C58" t="n">
-        <v>2.08</v>
+        <v>2.28</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" s="1" t="inlineStr">
         <is>
-          <t>PBR/SGML</t>
+          <t>PBR/SUZ</t>
         </is>
       </c>
       <c r="B59" s="11" t="inlineStr">
@@ -1522,13 +1498,13 @@
         </is>
       </c>
       <c r="C59" t="n">
-        <v>3.87</v>
+        <v>2.37</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" s="1" t="inlineStr">
         <is>
-          <t>PBR/CIG</t>
+          <t>PBR/SGML</t>
         </is>
       </c>
       <c r="B60" s="11" t="inlineStr">
@@ -1537,13 +1513,13 @@
         </is>
       </c>
       <c r="C60" t="n">
-        <v>2.11</v>
+        <v>3.74</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" s="1" t="inlineStr">
         <is>
-          <t>PBR/ELP</t>
+          <t>PBR/CIG</t>
         </is>
       </c>
       <c r="B61" s="11" t="inlineStr">
@@ -1552,28 +1528,28 @@
         </is>
       </c>
       <c r="C61" t="n">
-        <v>2.5</v>
+        <v>2.05</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" s="1" t="inlineStr">
         <is>
-          <t>UGP/TIMB</t>
-        </is>
-      </c>
-      <c r="B62" s="12" t="inlineStr">
-        <is>
-          <t>UGP</t>
+          <t>PBR/ELP</t>
+        </is>
+      </c>
+      <c r="B62" s="11" t="inlineStr">
+        <is>
+          <t>PBR</t>
         </is>
       </c>
       <c r="C62" t="n">
-        <v>2.07</v>
+        <v>2.66</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" s="1" t="inlineStr">
         <is>
-          <t>UGP/ABEV</t>
+          <t>UGP/VIV</t>
         </is>
       </c>
       <c r="B63" s="12" t="inlineStr">
@@ -1582,13 +1558,13 @@
         </is>
       </c>
       <c r="C63" t="n">
-        <v>2.3</v>
+        <v>2.21</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" s="1" t="inlineStr">
         <is>
-          <t>UGP/CSAN</t>
+          <t>UGP/TIMB</t>
         </is>
       </c>
       <c r="B64" s="12" t="inlineStr">
@@ -1597,13 +1573,13 @@
         </is>
       </c>
       <c r="C64" t="n">
-        <v>2.13</v>
+        <v>2.52</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" s="1" t="inlineStr">
         <is>
-          <t>UGP/BBD</t>
+          <t>UGP/ABEV</t>
         </is>
       </c>
       <c r="B65" s="12" t="inlineStr">
@@ -1612,13 +1588,13 @@
         </is>
       </c>
       <c r="C65" t="n">
-        <v>3.23</v>
+        <v>2.42</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" s="1" t="inlineStr">
         <is>
-          <t>UGP/BSBR</t>
+          <t>UGP/NTCO</t>
         </is>
       </c>
       <c r="B66" s="12" t="inlineStr">
@@ -1627,13 +1603,13 @@
         </is>
       </c>
       <c r="C66" t="n">
-        <v>2.51</v>
+        <v>2.11</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" s="1" t="inlineStr">
         <is>
-          <t>UGP/AZUL</t>
+          <t>UGP/CSAN</t>
         </is>
       </c>
       <c r="B67" s="12" t="inlineStr">
@@ -1642,13 +1618,13 @@
         </is>
       </c>
       <c r="C67" t="n">
-        <v>2.85</v>
+        <v>2.07</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" s="1" t="inlineStr">
         <is>
-          <t>UGP/GOL</t>
+          <t>UGP/BBD</t>
         </is>
       </c>
       <c r="B68" s="12" t="inlineStr">
@@ -1657,13 +1633,13 @@
         </is>
       </c>
       <c r="C68" t="n">
-        <v>4.26</v>
+        <v>3.24</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" s="1" t="inlineStr">
         <is>
-          <t>UGP/GGB</t>
+          <t>UGP/BSBR</t>
         </is>
       </c>
       <c r="B69" s="12" t="inlineStr">
@@ -1672,13 +1648,13 @@
         </is>
       </c>
       <c r="C69" t="n">
-        <v>2.39</v>
+        <v>2.42</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" s="1" t="inlineStr">
         <is>
-          <t>UGP/SUZ</t>
+          <t>UGP/AZUL</t>
         </is>
       </c>
       <c r="B70" s="12" t="inlineStr">
@@ -1687,13 +1663,13 @@
         </is>
       </c>
       <c r="C70" t="n">
-        <v>2.33</v>
+        <v>2.94</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" s="1" t="inlineStr">
         <is>
-          <t>UGP/BAK</t>
+          <t>UGP/GOL</t>
         </is>
       </c>
       <c r="B71" s="12" t="inlineStr">
@@ -1702,13 +1678,13 @@
         </is>
       </c>
       <c r="C71" t="n">
-        <v>2.25</v>
+        <v>4.45</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" s="1" t="inlineStr">
         <is>
-          <t>UGP/VALE</t>
+          <t>UGP/GGB</t>
         </is>
       </c>
       <c r="B72" s="12" t="inlineStr">
@@ -1717,13 +1693,13 @@
         </is>
       </c>
       <c r="C72" t="n">
-        <v>2.4</v>
+        <v>2.33</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" s="1" t="inlineStr">
         <is>
-          <t>UGP/SGML</t>
+          <t>UGP/SUZ</t>
         </is>
       </c>
       <c r="B73" s="12" t="inlineStr">
@@ -1732,13 +1708,13 @@
         </is>
       </c>
       <c r="C73" t="n">
-        <v>3.83</v>
+        <v>2.24</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" s="1" t="inlineStr">
         <is>
-          <t>UGP/CIG</t>
+          <t>UGP/VALE</t>
         </is>
       </c>
       <c r="B74" s="12" t="inlineStr">
@@ -1747,13 +1723,13 @@
         </is>
       </c>
       <c r="C74" t="n">
-        <v>2.13</v>
+        <v>2.25</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" s="1" t="inlineStr">
         <is>
-          <t>UGP/ELP</t>
+          <t>UGP/SGML</t>
         </is>
       </c>
       <c r="B75" s="12" t="inlineStr">
@@ -1762,58 +1738,58 @@
         </is>
       </c>
       <c r="C75" t="n">
-        <v>2.56</v>
+        <v>3.69</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" s="1" t="inlineStr">
         <is>
-          <t>BBD/VIV</t>
-        </is>
-      </c>
-      <c r="B76" s="13" t="inlineStr">
-        <is>
-          <t>BBD</t>
+          <t>UGP/EBR</t>
+        </is>
+      </c>
+      <c r="B76" s="12" t="inlineStr">
+        <is>
+          <t>UGP</t>
         </is>
       </c>
       <c r="C76" t="n">
-        <v>-2.69</v>
+        <v>2.05</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" s="1" t="inlineStr">
         <is>
-          <t>BBD/TIMB</t>
-        </is>
-      </c>
-      <c r="B77" s="13" t="inlineStr">
-        <is>
-          <t>BBD</t>
+          <t>UGP/CIG</t>
+        </is>
+      </c>
+      <c r="B77" s="12" t="inlineStr">
+        <is>
+          <t>UGP</t>
         </is>
       </c>
       <c r="C77" t="n">
-        <v>-2.61</v>
+        <v>2.06</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" s="1" t="inlineStr">
         <is>
-          <t>BBD/NTCO</t>
-        </is>
-      </c>
-      <c r="B78" s="13" t="inlineStr">
-        <is>
-          <t>BBD</t>
+          <t>UGP/ELP</t>
+        </is>
+      </c>
+      <c r="B78" s="12" t="inlineStr">
+        <is>
+          <t>UGP</t>
         </is>
       </c>
       <c r="C78" t="n">
-        <v>-2.01</v>
+        <v>2.63</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" s="1" t="inlineStr">
         <is>
-          <t>BBD/CSAN</t>
+          <t>BBD/VIV</t>
         </is>
       </c>
       <c r="B79" s="13" t="inlineStr">
@@ -1822,13 +1798,13 @@
         </is>
       </c>
       <c r="C79" t="n">
-        <v>-2.5</v>
+        <v>-2.47</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" s="1" t="inlineStr">
         <is>
-          <t>BBD/PBR</t>
+          <t>BBD/TIMB</t>
         </is>
       </c>
       <c r="B80" s="13" t="inlineStr">
@@ -1837,13 +1813,13 @@
         </is>
       </c>
       <c r="C80" t="n">
-        <v>-2.32</v>
+        <v>-2.31</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" s="1" t="inlineStr">
         <is>
-          <t>BBD/UGP</t>
+          <t>BBD/CSAN</t>
         </is>
       </c>
       <c r="B81" s="13" t="inlineStr">
@@ -1852,13 +1828,13 @@
         </is>
       </c>
       <c r="C81" t="n">
-        <v>-2.32</v>
+        <v>-2.64</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" s="1" t="inlineStr">
         <is>
-          <t>BBD/BSBR</t>
+          <t>BBD/PBR</t>
         </is>
       </c>
       <c r="B82" s="13" t="inlineStr">
@@ -1867,13 +1843,13 @@
         </is>
       </c>
       <c r="C82" t="n">
-        <v>-2.35</v>
+        <v>-2.36</v>
       </c>
     </row>
     <row r="83">
       <c r="A83" s="1" t="inlineStr">
         <is>
-          <t>BBD/ITUB</t>
+          <t>BBD/UGP</t>
         </is>
       </c>
       <c r="B83" s="13" t="inlineStr">
@@ -1882,13 +1858,13 @@
         </is>
       </c>
       <c r="C83" t="n">
-        <v>-3.45</v>
+        <v>-2.32</v>
       </c>
     </row>
     <row r="84">
       <c r="A84" s="1" t="inlineStr">
         <is>
-          <t>BBD/NU</t>
+          <t>BBD/BSBR</t>
         </is>
       </c>
       <c r="B84" s="13" t="inlineStr">
@@ -1897,13 +1873,13 @@
         </is>
       </c>
       <c r="C84" t="n">
-        <v>-2.35</v>
+        <v>-2.75</v>
       </c>
     </row>
     <row r="85">
       <c r="A85" s="1" t="inlineStr">
         <is>
-          <t>BBD/PAGS</t>
+          <t>BBD/ITUB</t>
         </is>
       </c>
       <c r="B85" s="13" t="inlineStr">
@@ -1912,13 +1888,13 @@
         </is>
       </c>
       <c r="C85" t="n">
-        <v>-2.64</v>
+        <v>-3.46</v>
       </c>
     </row>
     <row r="86">
       <c r="A86" s="1" t="inlineStr">
         <is>
-          <t>BBD/STNE</t>
+          <t>BBD/NU</t>
         </is>
       </c>
       <c r="B86" s="13" t="inlineStr">
@@ -1927,13 +1903,13 @@
         </is>
       </c>
       <c r="C86" t="n">
-        <v>-2.34</v>
+        <v>-2.29</v>
       </c>
     </row>
     <row r="87">
       <c r="A87" s="1" t="inlineStr">
         <is>
-          <t>BBD/ERJ</t>
+          <t>BBD/PAGS</t>
         </is>
       </c>
       <c r="B87" s="13" t="inlineStr">
@@ -1942,13 +1918,13 @@
         </is>
       </c>
       <c r="C87" t="n">
-        <v>-2.16</v>
+        <v>-2.44</v>
       </c>
     </row>
     <row r="88">
       <c r="A88" s="1" t="inlineStr">
         <is>
-          <t>BBD/GOL</t>
+          <t>BBD/STNE</t>
         </is>
       </c>
       <c r="B88" s="13" t="inlineStr">
@@ -1957,13 +1933,13 @@
         </is>
       </c>
       <c r="C88" t="n">
-        <v>3.58</v>
+        <v>-2.12</v>
       </c>
     </row>
     <row r="89">
       <c r="A89" s="1" t="inlineStr">
         <is>
-          <t>BBD/SGML</t>
+          <t>BBD/ERJ</t>
         </is>
       </c>
       <c r="B89" s="13" t="inlineStr">
@@ -1972,13 +1948,13 @@
         </is>
       </c>
       <c r="C89" t="n">
-        <v>3.2</v>
+        <v>-2.1</v>
       </c>
     </row>
     <row r="90">
       <c r="A90" s="1" t="inlineStr">
         <is>
-          <t>BBD/EBR</t>
+          <t>BBD/GOL</t>
         </is>
       </c>
       <c r="B90" s="13" t="inlineStr">
@@ -1987,13 +1963,13 @@
         </is>
       </c>
       <c r="C90" t="n">
-        <v>-3.74</v>
+        <v>3.78</v>
       </c>
     </row>
     <row r="91">
       <c r="A91" s="1" t="inlineStr">
         <is>
-          <t>BBD/SBS</t>
+          <t>BBD/SID</t>
         </is>
       </c>
       <c r="B91" s="13" t="inlineStr">
@@ -2002,58 +1978,58 @@
         </is>
       </c>
       <c r="C91" t="n">
-        <v>-2.58</v>
+        <v>-2.11</v>
       </c>
     </row>
     <row r="92">
       <c r="A92" s="1" t="inlineStr">
         <is>
-          <t>BSBR/VIV</t>
-        </is>
-      </c>
-      <c r="B92" s="14" t="inlineStr">
-        <is>
-          <t>BSBR</t>
+          <t>BBD/SGML</t>
+        </is>
+      </c>
+      <c r="B92" s="13" t="inlineStr">
+        <is>
+          <t>BBD</t>
         </is>
       </c>
       <c r="C92" t="n">
-        <v>-2.08</v>
+        <v>3.03</v>
       </c>
     </row>
     <row r="93">
       <c r="A93" s="1" t="inlineStr">
         <is>
-          <t>BSBR/BBD</t>
-        </is>
-      </c>
-      <c r="B93" s="14" t="inlineStr">
-        <is>
-          <t>BSBR</t>
+          <t>BBD/EBR</t>
+        </is>
+      </c>
+      <c r="B93" s="13" t="inlineStr">
+        <is>
+          <t>BBD</t>
         </is>
       </c>
       <c r="C93" t="n">
-        <v>2.52</v>
+        <v>-3.5</v>
       </c>
     </row>
     <row r="94">
       <c r="A94" s="1" t="inlineStr">
         <is>
-          <t>BSBR/ITUB</t>
-        </is>
-      </c>
-      <c r="B94" s="14" t="inlineStr">
-        <is>
-          <t>BSBR</t>
+          <t>BBD/SBS</t>
+        </is>
+      </c>
+      <c r="B94" s="13" t="inlineStr">
+        <is>
+          <t>BBD</t>
         </is>
       </c>
       <c r="C94" t="n">
-        <v>-2.53</v>
+        <v>-2.59</v>
       </c>
     </row>
     <row r="95">
       <c r="A95" s="1" t="inlineStr">
         <is>
-          <t>BSBR/PAGS</t>
+          <t>BSBR/BBD</t>
         </is>
       </c>
       <c r="B95" s="14" t="inlineStr">
@@ -2062,13 +2038,13 @@
         </is>
       </c>
       <c r="C95" t="n">
-        <v>-2.15</v>
+        <v>3.01</v>
       </c>
     </row>
     <row r="96">
       <c r="A96" s="1" t="inlineStr">
         <is>
-          <t>BSBR/GOL</t>
+          <t>BSBR/ITUB</t>
         </is>
       </c>
       <c r="B96" s="14" t="inlineStr">
@@ -2077,13 +2053,13 @@
         </is>
       </c>
       <c r="C96" t="n">
-        <v>4</v>
+        <v>-2.4</v>
       </c>
     </row>
     <row r="97">
       <c r="A97" s="1" t="inlineStr">
         <is>
-          <t>BSBR/SGML</t>
+          <t>BSBR/GOL</t>
         </is>
       </c>
       <c r="B97" s="14" t="inlineStr">
@@ -2092,13 +2068,13 @@
         </is>
       </c>
       <c r="C97" t="n">
-        <v>3.74</v>
+        <v>4.31</v>
       </c>
     </row>
     <row r="98">
       <c r="A98" s="1" t="inlineStr">
         <is>
-          <t>BSBR/EBR</t>
+          <t>BSBR/SGML</t>
         </is>
       </c>
       <c r="B98" s="14" t="inlineStr">
@@ -2107,13 +2083,13 @@
         </is>
       </c>
       <c r="C98" t="n">
-        <v>-2.73</v>
+        <v>3.65</v>
       </c>
     </row>
     <row r="99">
       <c r="A99" s="1" t="inlineStr">
         <is>
-          <t>BSBR/SBS</t>
+          <t>BSBR/EBR</t>
         </is>
       </c>
       <c r="B99" s="14" t="inlineStr">
@@ -2122,28 +2098,28 @@
         </is>
       </c>
       <c r="C99" t="n">
-        <v>-2.1</v>
+        <v>-2.19</v>
       </c>
     </row>
     <row r="100">
       <c r="A100" s="1" t="inlineStr">
         <is>
-          <t>ITUB/ABEV</t>
-        </is>
-      </c>
-      <c r="B100" s="15" t="inlineStr">
-        <is>
-          <t>ITUB</t>
+          <t>BSBR/SBS</t>
+        </is>
+      </c>
+      <c r="B100" s="14" t="inlineStr">
+        <is>
+          <t>BSBR</t>
         </is>
       </c>
       <c r="C100" t="n">
-        <v>2.36</v>
+        <v>-2.04</v>
       </c>
     </row>
     <row r="101">
       <c r="A101" s="1" t="inlineStr">
         <is>
-          <t>ITUB/BBD</t>
+          <t>ITUB/ABEV</t>
         </is>
       </c>
       <c r="B101" s="15" t="inlineStr">
@@ -2152,13 +2128,13 @@
         </is>
       </c>
       <c r="C101" t="n">
-        <v>4.16</v>
+        <v>2.57</v>
       </c>
     </row>
     <row r="102">
       <c r="A102" s="1" t="inlineStr">
         <is>
-          <t>ITUB/BSBR</t>
+          <t>ITUB/BBD</t>
         </is>
       </c>
       <c r="B102" s="15" t="inlineStr">
@@ -2167,13 +2143,13 @@
         </is>
       </c>
       <c r="C102" t="n">
-        <v>2.91</v>
+        <v>4.17</v>
       </c>
     </row>
     <row r="103">
       <c r="A103" s="1" t="inlineStr">
         <is>
-          <t>ITUB/AZUL</t>
+          <t>ITUB/BSBR</t>
         </is>
       </c>
       <c r="B103" s="15" t="inlineStr">
@@ -2182,13 +2158,13 @@
         </is>
       </c>
       <c r="C103" t="n">
-        <v>2.12</v>
+        <v>2.72</v>
       </c>
     </row>
     <row r="104">
       <c r="A104" s="1" t="inlineStr">
         <is>
-          <t>ITUB/GOL</t>
+          <t>ITUB/AZUL</t>
         </is>
       </c>
       <c r="B104" s="15" t="inlineStr">
@@ -2197,13 +2173,13 @@
         </is>
       </c>
       <c r="C104" t="n">
-        <v>4.24</v>
+        <v>2.34</v>
       </c>
     </row>
     <row r="105">
       <c r="A105" s="1" t="inlineStr">
         <is>
-          <t>ITUB/GGB</t>
+          <t>ITUB/GOL</t>
         </is>
       </c>
       <c r="B105" s="15" t="inlineStr">
@@ -2212,13 +2188,13 @@
         </is>
       </c>
       <c r="C105" t="n">
-        <v>2.44</v>
+        <v>4.45</v>
       </c>
     </row>
     <row r="106">
       <c r="A106" s="1" t="inlineStr">
         <is>
-          <t>ITUB/BAK</t>
+          <t>ITUB/GGB</t>
         </is>
       </c>
       <c r="B106" s="15" t="inlineStr">
@@ -2227,7 +2203,7 @@
         </is>
       </c>
       <c r="C106" t="n">
-        <v>2.12</v>
+        <v>2.36</v>
       </c>
     </row>
     <row r="107">
@@ -2242,7 +2218,7 @@
         </is>
       </c>
       <c r="C107" t="n">
-        <v>2.21</v>
+        <v>2</v>
       </c>
     </row>
     <row r="108">
@@ -2257,7 +2233,7 @@
         </is>
       </c>
       <c r="C108" t="n">
-        <v>3.95</v>
+        <v>3.79</v>
       </c>
     </row>
     <row r="109">
@@ -2272,13 +2248,13 @@
         </is>
       </c>
       <c r="C109" t="n">
-        <v>2.28</v>
+        <v>2.44</v>
       </c>
     </row>
     <row r="110">
       <c r="A110" s="1" t="inlineStr">
         <is>
-          <t>NU/ABEV</t>
+          <t>NU/TIMB</t>
         </is>
       </c>
       <c r="B110" s="16" t="inlineStr">
@@ -2287,13 +2263,13 @@
         </is>
       </c>
       <c r="C110" t="n">
-        <v>2.58</v>
+        <v>2.07</v>
       </c>
     </row>
     <row r="111">
       <c r="A111" s="1" t="inlineStr">
         <is>
-          <t>NU/CSAN</t>
+          <t>NU/ABEV</t>
         </is>
       </c>
       <c r="B111" s="16" t="inlineStr">
@@ -2302,13 +2278,13 @@
         </is>
       </c>
       <c r="C111" t="n">
-        <v>2.42</v>
+        <v>2.57</v>
       </c>
     </row>
     <row r="112">
       <c r="A112" s="1" t="inlineStr">
         <is>
-          <t>NU/BBD</t>
+          <t>NU/NTCO</t>
         </is>
       </c>
       <c r="B112" s="16" t="inlineStr">
@@ -2317,13 +2293,13 @@
         </is>
       </c>
       <c r="C112" t="n">
-        <v>3.67</v>
+        <v>2.13</v>
       </c>
     </row>
     <row r="113">
       <c r="A113" s="1" t="inlineStr">
         <is>
-          <t>NU/BSBR</t>
+          <t>NU/CSAN</t>
         </is>
       </c>
       <c r="B113" s="16" t="inlineStr">
@@ -2332,13 +2308,13 @@
         </is>
       </c>
       <c r="C113" t="n">
-        <v>2.63</v>
+        <v>2.17</v>
       </c>
     </row>
     <row r="114">
       <c r="A114" s="1" t="inlineStr">
         <is>
-          <t>NU/AZUL</t>
+          <t>NU/BBD</t>
         </is>
       </c>
       <c r="B114" s="16" t="inlineStr">
@@ -2347,13 +2323,13 @@
         </is>
       </c>
       <c r="C114" t="n">
-        <v>3.29</v>
+        <v>3.49</v>
       </c>
     </row>
     <row r="115">
       <c r="A115" s="1" t="inlineStr">
         <is>
-          <t>NU/GOL</t>
+          <t>NU/BSBR</t>
         </is>
       </c>
       <c r="B115" s="16" t="inlineStr">
@@ -2362,13 +2338,13 @@
         </is>
       </c>
       <c r="C115" t="n">
-        <v>4.72</v>
+        <v>2.37</v>
       </c>
     </row>
     <row r="116">
       <c r="A116" s="1" t="inlineStr">
         <is>
-          <t>NU/GGB</t>
+          <t>NU/AZUL</t>
         </is>
       </c>
       <c r="B116" s="16" t="inlineStr">
@@ -2377,13 +2353,13 @@
         </is>
       </c>
       <c r="C116" t="n">
-        <v>2.75</v>
+        <v>3.25</v>
       </c>
     </row>
     <row r="117">
       <c r="A117" s="1" t="inlineStr">
         <is>
-          <t>NU/SUZ</t>
+          <t>NU/GOL</t>
         </is>
       </c>
       <c r="B117" s="16" t="inlineStr">
@@ -2392,13 +2368,13 @@
         </is>
       </c>
       <c r="C117" t="n">
-        <v>2.6</v>
+        <v>4.76</v>
       </c>
     </row>
     <row r="118">
       <c r="A118" s="1" t="inlineStr">
         <is>
-          <t>NU/BAK</t>
+          <t>NU/GGB</t>
         </is>
       </c>
       <c r="B118" s="16" t="inlineStr">
@@ -2407,13 +2383,13 @@
         </is>
       </c>
       <c r="C118" t="n">
-        <v>2.62</v>
+        <v>2.55</v>
       </c>
     </row>
     <row r="119">
       <c r="A119" s="1" t="inlineStr">
         <is>
-          <t>NU/VALE</t>
+          <t>NU/SUZ</t>
         </is>
       </c>
       <c r="B119" s="16" t="inlineStr">
@@ -2422,13 +2398,13 @@
         </is>
       </c>
       <c r="C119" t="n">
-        <v>2.4</v>
+        <v>2.31</v>
       </c>
     </row>
     <row r="120">
       <c r="A120" s="1" t="inlineStr">
         <is>
-          <t>NU/SGML</t>
+          <t>NU/VALE</t>
         </is>
       </c>
       <c r="B120" s="16" t="inlineStr">
@@ -2437,13 +2413,13 @@
         </is>
       </c>
       <c r="C120" t="n">
-        <v>4.23</v>
+        <v>2.12</v>
       </c>
     </row>
     <row r="121">
       <c r="A121" s="1" t="inlineStr">
         <is>
-          <t>NU/CIG</t>
+          <t>NU/SGML</t>
         </is>
       </c>
       <c r="B121" s="16" t="inlineStr">
@@ -2452,13 +2428,13 @@
         </is>
       </c>
       <c r="C121" t="n">
-        <v>2.56</v>
+        <v>3.93</v>
       </c>
     </row>
     <row r="122">
       <c r="A122" s="1" t="inlineStr">
         <is>
-          <t>NU/ELP</t>
+          <t>NU/CIG</t>
         </is>
       </c>
       <c r="B122" s="16" t="inlineStr">
@@ -2467,28 +2443,28 @@
         </is>
       </c>
       <c r="C122" t="n">
-        <v>2.88</v>
+        <v>2.32</v>
       </c>
     </row>
     <row r="123">
       <c r="A123" s="1" t="inlineStr">
         <is>
-          <t>PAGS/ABEV</t>
-        </is>
-      </c>
-      <c r="B123" s="17" t="inlineStr">
-        <is>
-          <t>PAGS</t>
+          <t>NU/ELP</t>
+        </is>
+      </c>
+      <c r="B123" s="16" t="inlineStr">
+        <is>
+          <t>NU</t>
         </is>
       </c>
       <c r="C123" t="n">
-        <v>2.63</v>
+        <v>2.78</v>
       </c>
     </row>
     <row r="124">
       <c r="A124" s="1" t="inlineStr">
         <is>
-          <t>PAGS/BBD</t>
+          <t>PAGS/ABEV</t>
         </is>
       </c>
       <c r="B124" s="17" t="inlineStr">
@@ -2497,13 +2473,13 @@
         </is>
       </c>
       <c r="C124" t="n">
-        <v>3.47</v>
+        <v>2.43</v>
       </c>
     </row>
     <row r="125">
       <c r="A125" s="1" t="inlineStr">
         <is>
-          <t>PAGS/BSBR</t>
+          <t>PAGS/BBD</t>
         </is>
       </c>
       <c r="B125" s="17" t="inlineStr">
@@ -2512,13 +2488,13 @@
         </is>
       </c>
       <c r="C125" t="n">
-        <v>2.66</v>
+        <v>3.06</v>
       </c>
     </row>
     <row r="126">
       <c r="A126" s="1" t="inlineStr">
         <is>
-          <t>PAGS/AZUL</t>
+          <t>PAGS/BSBR</t>
         </is>
       </c>
       <c r="B126" s="17" t="inlineStr">
@@ -2527,13 +2503,13 @@
         </is>
       </c>
       <c r="C126" t="n">
-        <v>2.24</v>
+        <v>2.12</v>
       </c>
     </row>
     <row r="127">
       <c r="A127" s="1" t="inlineStr">
         <is>
-          <t>PAGS/GOL</t>
+          <t>PAGS/AZUL</t>
         </is>
       </c>
       <c r="B127" s="17" t="inlineStr">
@@ -2542,13 +2518,13 @@
         </is>
       </c>
       <c r="C127" t="n">
-        <v>4.14</v>
+        <v>2.12</v>
       </c>
     </row>
     <row r="128">
       <c r="A128" s="1" t="inlineStr">
         <is>
-          <t>PAGS/GGB</t>
+          <t>PAGS/GOL</t>
         </is>
       </c>
       <c r="B128" s="17" t="inlineStr">
@@ -2557,13 +2533,13 @@
         </is>
       </c>
       <c r="C128" t="n">
-        <v>2.66</v>
+        <v>4.08</v>
       </c>
     </row>
     <row r="129">
       <c r="A129" s="1" t="inlineStr">
         <is>
-          <t>PAGS/BAK</t>
+          <t>PAGS/GGB</t>
         </is>
       </c>
       <c r="B129" s="17" t="inlineStr">
@@ -2572,13 +2548,13 @@
         </is>
       </c>
       <c r="C129" t="n">
-        <v>2.58</v>
+        <v>2.27</v>
       </c>
     </row>
     <row r="130">
       <c r="A130" s="1" t="inlineStr">
         <is>
-          <t>PAGS/VALE</t>
+          <t>PAGS/SGML</t>
         </is>
       </c>
       <c r="B130" s="17" t="inlineStr">
@@ -2587,783 +2563,783 @@
         </is>
       </c>
       <c r="C130" t="n">
-        <v>2.42</v>
+        <v>3.73</v>
       </c>
     </row>
     <row r="131">
       <c r="A131" s="1" t="inlineStr">
         <is>
-          <t>PAGS/SGML</t>
-        </is>
-      </c>
-      <c r="B131" s="17" t="inlineStr">
-        <is>
-          <t>PAGS</t>
+          <t>ERJ/ABEV</t>
+        </is>
+      </c>
+      <c r="B131" s="18" t="inlineStr">
+        <is>
+          <t>ERJ</t>
         </is>
       </c>
       <c r="C131" t="n">
-        <v>4.18</v>
+        <v>2.32</v>
       </c>
     </row>
     <row r="132">
       <c r="A132" s="1" t="inlineStr">
         <is>
-          <t>PAGS/CIG</t>
-        </is>
-      </c>
-      <c r="B132" s="17" t="inlineStr">
-        <is>
-          <t>PAGS</t>
+          <t>ERJ/BBD</t>
+        </is>
+      </c>
+      <c r="B132" s="18" t="inlineStr">
+        <is>
+          <t>ERJ</t>
         </is>
       </c>
       <c r="C132" t="n">
-        <v>2.13</v>
+        <v>2.5</v>
       </c>
     </row>
     <row r="133">
       <c r="A133" s="1" t="inlineStr">
         <is>
-          <t>STNE/ABEV</t>
+          <t>ERJ/GOL</t>
         </is>
       </c>
       <c r="B133" s="18" t="inlineStr">
         <is>
-          <t>STNE</t>
+          <t>ERJ</t>
         </is>
       </c>
       <c r="C133" t="n">
-        <v>2.04</v>
+        <v>4.21</v>
       </c>
     </row>
     <row r="134">
       <c r="A134" s="1" t="inlineStr">
         <is>
-          <t>STNE/BBD</t>
+          <t>ERJ/GGB</t>
         </is>
       </c>
       <c r="B134" s="18" t="inlineStr">
         <is>
-          <t>STNE</t>
+          <t>ERJ</t>
         </is>
       </c>
       <c r="C134" t="n">
-        <v>2.94</v>
+        <v>2.07</v>
       </c>
     </row>
     <row r="135">
       <c r="A135" s="1" t="inlineStr">
         <is>
-          <t>STNE/BSBR</t>
+          <t>ERJ/VALE</t>
         </is>
       </c>
       <c r="B135" s="18" t="inlineStr">
         <is>
-          <t>STNE</t>
+          <t>ERJ</t>
         </is>
       </c>
       <c r="C135" t="n">
-        <v>2.11</v>
+        <v>2.02</v>
       </c>
     </row>
     <row r="136">
       <c r="A136" s="1" t="inlineStr">
         <is>
-          <t>STNE/AZUL</t>
+          <t>ERJ/SGML</t>
         </is>
       </c>
       <c r="B136" s="18" t="inlineStr">
         <is>
-          <t>STNE</t>
+          <t>ERJ</t>
         </is>
       </c>
       <c r="C136" t="n">
-        <v>2.32</v>
+        <v>3.75</v>
       </c>
     </row>
     <row r="137">
       <c r="A137" s="1" t="inlineStr">
         <is>
-          <t>STNE/GOL</t>
-        </is>
-      </c>
-      <c r="B137" s="18" t="inlineStr">
-        <is>
-          <t>STNE</t>
+          <t>GOL/VIV</t>
+        </is>
+      </c>
+      <c r="B137" s="19" t="inlineStr">
+        <is>
+          <t>GOL</t>
         </is>
       </c>
       <c r="C137" t="n">
-        <v>3.93</v>
+        <v>-2.6</v>
       </c>
     </row>
     <row r="138">
       <c r="A138" s="1" t="inlineStr">
         <is>
-          <t>STNE/GGB</t>
-        </is>
-      </c>
-      <c r="B138" s="18" t="inlineStr">
-        <is>
-          <t>STNE</t>
+          <t>GOL/TIMB</t>
+        </is>
+      </c>
+      <c r="B138" s="19" t="inlineStr">
+        <is>
+          <t>GOL</t>
         </is>
       </c>
       <c r="C138" t="n">
-        <v>2.11</v>
+        <v>-2.56</v>
       </c>
     </row>
     <row r="139">
       <c r="A139" s="1" t="inlineStr">
         <is>
-          <t>STNE/BAK</t>
-        </is>
-      </c>
-      <c r="B139" s="18" t="inlineStr">
-        <is>
-          <t>STNE</t>
+          <t>GOL/ABEV</t>
+        </is>
+      </c>
+      <c r="B139" s="19" t="inlineStr">
+        <is>
+          <t>GOL</t>
         </is>
       </c>
       <c r="C139" t="n">
-        <v>2.05</v>
+        <v>-2.74</v>
       </c>
     </row>
     <row r="140">
       <c r="A140" s="1" t="inlineStr">
         <is>
-          <t>STNE/SGML</t>
-        </is>
-      </c>
-      <c r="B140" s="18" t="inlineStr">
-        <is>
-          <t>STNE</t>
+          <t>GOL/BRFS</t>
+        </is>
+      </c>
+      <c r="B140" s="19" t="inlineStr">
+        <is>
+          <t>GOL</t>
         </is>
       </c>
       <c r="C140" t="n">
-        <v>3.69</v>
+        <v>-2.37</v>
       </c>
     </row>
     <row r="141">
       <c r="A141" s="1" t="inlineStr">
         <is>
-          <t>ERJ/ABEV</t>
+          <t>GOL/NTCO</t>
         </is>
       </c>
       <c r="B141" s="19" t="inlineStr">
         <is>
-          <t>ERJ</t>
+          <t>GOL</t>
         </is>
       </c>
       <c r="C141" t="n">
-        <v>2.26</v>
+        <v>-3.01</v>
       </c>
     </row>
     <row r="142">
       <c r="A142" s="1" t="inlineStr">
         <is>
-          <t>ERJ/BBD</t>
+          <t>GOL/ASAI</t>
         </is>
       </c>
       <c r="B142" s="19" t="inlineStr">
         <is>
-          <t>ERJ</t>
+          <t>GOL</t>
         </is>
       </c>
       <c r="C142" t="n">
-        <v>2.6</v>
+        <v>-2.55</v>
       </c>
     </row>
     <row r="143">
       <c r="A143" s="1" t="inlineStr">
         <is>
-          <t>ERJ/GOL</t>
+          <t>GOL/CSAN</t>
         </is>
       </c>
       <c r="B143" s="19" t="inlineStr">
         <is>
-          <t>ERJ</t>
+          <t>GOL</t>
         </is>
       </c>
       <c r="C143" t="n">
-        <v>4.09</v>
+        <v>-2.98</v>
       </c>
     </row>
     <row r="144">
       <c r="A144" s="1" t="inlineStr">
         <is>
-          <t>ERJ/GGB</t>
+          <t>GOL/PBR</t>
         </is>
       </c>
       <c r="B144" s="19" t="inlineStr">
         <is>
-          <t>ERJ</t>
+          <t>GOL</t>
         </is>
       </c>
       <c r="C144" t="n">
-        <v>2.28</v>
+        <v>-2.66</v>
       </c>
     </row>
     <row r="145">
       <c r="A145" s="1" t="inlineStr">
         <is>
-          <t>ERJ/VALE</t>
+          <t>GOL/UGP</t>
         </is>
       </c>
       <c r="B145" s="19" t="inlineStr">
         <is>
-          <t>ERJ</t>
+          <t>GOL</t>
         </is>
       </c>
       <c r="C145" t="n">
-        <v>2.46</v>
+        <v>-2.56</v>
       </c>
     </row>
     <row r="146">
       <c r="A146" s="1" t="inlineStr">
         <is>
-          <t>ERJ/SGML</t>
+          <t>GOL/BBD</t>
         </is>
       </c>
       <c r="B146" s="19" t="inlineStr">
         <is>
-          <t>ERJ</t>
+          <t>GOL</t>
         </is>
       </c>
       <c r="C146" t="n">
-        <v>4.02</v>
+        <v>-2.9</v>
       </c>
     </row>
     <row r="147">
       <c r="A147" s="1" t="inlineStr">
         <is>
-          <t>GOL/VIV</t>
-        </is>
-      </c>
-      <c r="B147" s="20" t="inlineStr">
+          <t>GOL/BSBR</t>
+        </is>
+      </c>
+      <c r="B147" s="19" t="inlineStr">
         <is>
           <t>GOL</t>
         </is>
       </c>
       <c r="C147" t="n">
-        <v>-2.61</v>
+        <v>-2.92</v>
       </c>
     </row>
     <row r="148">
       <c r="A148" s="1" t="inlineStr">
         <is>
-          <t>GOL/TIMB</t>
-        </is>
-      </c>
-      <c r="B148" s="20" t="inlineStr">
+          <t>GOL/ITUB</t>
+        </is>
+      </c>
+      <c r="B148" s="19" t="inlineStr">
         <is>
           <t>GOL</t>
         </is>
       </c>
       <c r="C148" t="n">
-        <v>-2.59</v>
+        <v>-2.84</v>
       </c>
     </row>
     <row r="149">
       <c r="A149" s="1" t="inlineStr">
         <is>
-          <t>GOL/ABEV</t>
-        </is>
-      </c>
-      <c r="B149" s="20" t="inlineStr">
+          <t>GOL/NU</t>
+        </is>
+      </c>
+      <c r="B149" s="19" t="inlineStr">
         <is>
           <t>GOL</t>
         </is>
       </c>
       <c r="C149" t="n">
-        <v>-2.72</v>
+        <v>-2.84</v>
       </c>
     </row>
     <row r="150">
       <c r="A150" s="1" t="inlineStr">
         <is>
-          <t>GOL/BRFS</t>
-        </is>
-      </c>
-      <c r="B150" s="20" t="inlineStr">
+          <t>GOL/PAGS</t>
+        </is>
+      </c>
+      <c r="B150" s="19" t="inlineStr">
         <is>
           <t>GOL</t>
         </is>
       </c>
       <c r="C150" t="n">
-        <v>-2.37</v>
+        <v>-2.55</v>
       </c>
     </row>
     <row r="151">
       <c r="A151" s="1" t="inlineStr">
         <is>
-          <t>GOL/NTCO</t>
-        </is>
-      </c>
-      <c r="B151" s="20" t="inlineStr">
+          <t>GOL/STNE</t>
+        </is>
+      </c>
+      <c r="B151" s="19" t="inlineStr">
         <is>
           <t>GOL</t>
         </is>
       </c>
       <c r="C151" t="n">
-        <v>-3.05</v>
+        <v>-2.56</v>
       </c>
     </row>
     <row r="152">
       <c r="A152" s="1" t="inlineStr">
         <is>
-          <t>GOL/ASAI</t>
-        </is>
-      </c>
-      <c r="B152" s="20" t="inlineStr">
+          <t>GOL/XP</t>
+        </is>
+      </c>
+      <c r="B152" s="19" t="inlineStr">
         <is>
           <t>GOL</t>
         </is>
       </c>
       <c r="C152" t="n">
-        <v>-2.5</v>
+        <v>-2.4</v>
       </c>
     </row>
     <row r="153">
       <c r="A153" s="1" t="inlineStr">
         <is>
-          <t>GOL/CSAN</t>
-        </is>
-      </c>
-      <c r="B153" s="20" t="inlineStr">
+          <t>GOL/AZUL</t>
+        </is>
+      </c>
+      <c r="B153" s="19" t="inlineStr">
         <is>
           <t>GOL</t>
         </is>
       </c>
       <c r="C153" t="n">
-        <v>-2.95</v>
+        <v>-3.57</v>
       </c>
     </row>
     <row r="154">
       <c r="A154" s="1" t="inlineStr">
         <is>
-          <t>GOL/PBR</t>
-        </is>
-      </c>
-      <c r="B154" s="20" t="inlineStr">
+          <t>GOL/ERJ</t>
+        </is>
+      </c>
+      <c r="B154" s="19" t="inlineStr">
         <is>
           <t>GOL</t>
         </is>
       </c>
       <c r="C154" t="n">
-        <v>-2.64</v>
+        <v>-2.49</v>
       </c>
     </row>
     <row r="155">
       <c r="A155" s="1" t="inlineStr">
         <is>
-          <t>GOL/UGP</t>
-        </is>
-      </c>
-      <c r="B155" s="20" t="inlineStr">
+          <t>GOL/SID</t>
+        </is>
+      </c>
+      <c r="B155" s="19" t="inlineStr">
         <is>
           <t>GOL</t>
         </is>
       </c>
       <c r="C155" t="n">
-        <v>-2.56</v>
+        <v>-2.39</v>
       </c>
     </row>
     <row r="156">
       <c r="A156" s="1" t="inlineStr">
         <is>
-          <t>GOL/BBD</t>
-        </is>
-      </c>
-      <c r="B156" s="20" t="inlineStr">
+          <t>GOL/GGB</t>
+        </is>
+      </c>
+      <c r="B156" s="19" t="inlineStr">
         <is>
           <t>GOL</t>
         </is>
       </c>
       <c r="C156" t="n">
-        <v>-2.86</v>
+        <v>-2.58</v>
       </c>
     </row>
     <row r="157">
       <c r="A157" s="1" t="inlineStr">
         <is>
-          <t>GOL/BSBR</t>
-        </is>
-      </c>
-      <c r="B157" s="20" t="inlineStr">
+          <t>GOL/SUZ</t>
+        </is>
+      </c>
+      <c r="B157" s="19" t="inlineStr">
         <is>
           <t>GOL</t>
         </is>
       </c>
       <c r="C157" t="n">
-        <v>-2.85</v>
+        <v>-2.42</v>
       </c>
     </row>
     <row r="158">
       <c r="A158" s="1" t="inlineStr">
         <is>
-          <t>GOL/ITUB</t>
-        </is>
-      </c>
-      <c r="B158" s="20" t="inlineStr">
+          <t>GOL/BAK</t>
+        </is>
+      </c>
+      <c r="B158" s="19" t="inlineStr">
         <is>
           <t>GOL</t>
         </is>
       </c>
       <c r="C158" t="n">
-        <v>-2.82</v>
+        <v>-3.1</v>
       </c>
     </row>
     <row r="159">
       <c r="A159" s="1" t="inlineStr">
         <is>
-          <t>GOL/NU</t>
-        </is>
-      </c>
-      <c r="B159" s="20" t="inlineStr">
+          <t>GOL/VALE</t>
+        </is>
+      </c>
+      <c r="B159" s="19" t="inlineStr">
         <is>
           <t>GOL</t>
         </is>
       </c>
       <c r="C159" t="n">
-        <v>-2.86</v>
+        <v>-2.29</v>
       </c>
     </row>
     <row r="160">
       <c r="A160" s="1" t="inlineStr">
         <is>
-          <t>GOL/PAGS</t>
-        </is>
-      </c>
-      <c r="B160" s="20" t="inlineStr">
+          <t>GOL/EBR</t>
+        </is>
+      </c>
+      <c r="B160" s="19" t="inlineStr">
         <is>
           <t>GOL</t>
         </is>
       </c>
       <c r="C160" t="n">
-        <v>-2.57</v>
+        <v>-2.96</v>
       </c>
     </row>
     <row r="161">
       <c r="A161" s="1" t="inlineStr">
         <is>
-          <t>GOL/STNE</t>
-        </is>
-      </c>
-      <c r="B161" s="20" t="inlineStr">
+          <t>GOL/CIG</t>
+        </is>
+      </c>
+      <c r="B161" s="19" t="inlineStr">
         <is>
           <t>GOL</t>
         </is>
       </c>
       <c r="C161" t="n">
-        <v>-2.6</v>
+        <v>-2.7</v>
       </c>
     </row>
     <row r="162">
       <c r="A162" s="1" t="inlineStr">
         <is>
-          <t>GOL/XP</t>
-        </is>
-      </c>
-      <c r="B162" s="20" t="inlineStr">
+          <t>GOL/ELP</t>
+        </is>
+      </c>
+      <c r="B162" s="19" t="inlineStr">
         <is>
           <t>GOL</t>
         </is>
       </c>
       <c r="C162" t="n">
-        <v>-2.41</v>
+        <v>-2.55</v>
       </c>
     </row>
     <row r="163">
       <c r="A163" s="1" t="inlineStr">
         <is>
-          <t>GOL/AZUL</t>
-        </is>
-      </c>
-      <c r="B163" s="20" t="inlineStr">
+          <t>GOL/SBS</t>
+        </is>
+      </c>
+      <c r="B163" s="19" t="inlineStr">
         <is>
           <t>GOL</t>
         </is>
       </c>
       <c r="C163" t="n">
-        <v>-3.51</v>
+        <v>-2.56</v>
       </c>
     </row>
     <row r="164">
       <c r="A164" s="1" t="inlineStr">
         <is>
-          <t>GOL/ERJ</t>
+          <t>SID/ABEV</t>
         </is>
       </c>
       <c r="B164" s="20" t="inlineStr">
         <is>
-          <t>GOL</t>
+          <t>SID</t>
         </is>
       </c>
       <c r="C164" t="n">
-        <v>-2.48</v>
+        <v>2.44</v>
       </c>
     </row>
     <row r="165">
       <c r="A165" s="1" t="inlineStr">
         <is>
-          <t>GOL/SID</t>
+          <t>SID/BBD</t>
         </is>
       </c>
       <c r="B165" s="20" t="inlineStr">
         <is>
-          <t>GOL</t>
+          <t>SID</t>
         </is>
       </c>
       <c r="C165" t="n">
-        <v>-2.34</v>
+        <v>2.71</v>
       </c>
     </row>
     <row r="166">
       <c r="A166" s="1" t="inlineStr">
         <is>
-          <t>GOL/GGB</t>
+          <t>SID/BSBR</t>
         </is>
       </c>
       <c r="B166" s="20" t="inlineStr">
         <is>
-          <t>GOL</t>
+          <t>SID</t>
         </is>
       </c>
       <c r="C166" t="n">
-        <v>-2.49</v>
+        <v>2.1</v>
       </c>
     </row>
     <row r="167">
       <c r="A167" s="1" t="inlineStr">
         <is>
-          <t>GOL/SUZ</t>
+          <t>SID/GOL</t>
         </is>
       </c>
       <c r="B167" s="20" t="inlineStr">
         <is>
-          <t>GOL</t>
+          <t>SID</t>
         </is>
       </c>
       <c r="C167" t="n">
-        <v>-2.37</v>
+        <v>4.5</v>
       </c>
     </row>
     <row r="168">
       <c r="A168" s="1" t="inlineStr">
         <is>
-          <t>GOL/BAK</t>
+          <t>SID/GGB</t>
         </is>
       </c>
       <c r="B168" s="20" t="inlineStr">
         <is>
-          <t>GOL</t>
+          <t>SID</t>
         </is>
       </c>
       <c r="C168" t="n">
-        <v>-2.86</v>
+        <v>2.39</v>
       </c>
     </row>
     <row r="169">
       <c r="A169" s="1" t="inlineStr">
         <is>
-          <t>GOL/VALE</t>
+          <t>SID/VALE</t>
         </is>
       </c>
       <c r="B169" s="20" t="inlineStr">
         <is>
-          <t>GOL</t>
+          <t>SID</t>
         </is>
       </c>
       <c r="C169" t="n">
-        <v>-2.2</v>
+        <v>2.75</v>
       </c>
     </row>
     <row r="170">
       <c r="A170" s="1" t="inlineStr">
         <is>
-          <t>GOL/EBR</t>
+          <t>SID/SGML</t>
         </is>
       </c>
       <c r="B170" s="20" t="inlineStr">
         <is>
-          <t>GOL</t>
+          <t>SID</t>
         </is>
       </c>
       <c r="C170" t="n">
-        <v>-2.96</v>
+        <v>4.03</v>
       </c>
     </row>
     <row r="171">
       <c r="A171" s="1" t="inlineStr">
         <is>
-          <t>GOL/CIG</t>
-        </is>
-      </c>
-      <c r="B171" s="20" t="inlineStr">
-        <is>
-          <t>GOL</t>
+          <t>SGML/VIV</t>
+        </is>
+      </c>
+      <c r="B171" s="21" t="inlineStr">
+        <is>
+          <t>SGML</t>
         </is>
       </c>
       <c r="C171" t="n">
-        <v>-2.64</v>
+        <v>-2.3</v>
       </c>
     </row>
     <row r="172">
       <c r="A172" s="1" t="inlineStr">
         <is>
-          <t>GOL/ELP</t>
-        </is>
-      </c>
-      <c r="B172" s="20" t="inlineStr">
-        <is>
-          <t>GOL</t>
+          <t>SGML/TIMB</t>
+        </is>
+      </c>
+      <c r="B172" s="21" t="inlineStr">
+        <is>
+          <t>SGML</t>
         </is>
       </c>
       <c r="C172" t="n">
-        <v>-2.53</v>
+        <v>-2.22</v>
       </c>
     </row>
     <row r="173">
       <c r="A173" s="1" t="inlineStr">
         <is>
-          <t>GOL/SBS</t>
-        </is>
-      </c>
-      <c r="B173" s="20" t="inlineStr">
-        <is>
-          <t>GOL</t>
+          <t>SGML/ABEV</t>
+        </is>
+      </c>
+      <c r="B173" s="21" t="inlineStr">
+        <is>
+          <t>SGML</t>
         </is>
       </c>
       <c r="C173" t="n">
-        <v>-2.54</v>
+        <v>-2.91</v>
       </c>
     </row>
     <row r="174">
       <c r="A174" s="1" t="inlineStr">
         <is>
-          <t>SID/ABEV</t>
+          <t>SGML/NTCO</t>
         </is>
       </c>
       <c r="B174" s="21" t="inlineStr">
         <is>
-          <t>SID</t>
+          <t>SGML</t>
         </is>
       </c>
       <c r="C174" t="n">
-        <v>2.11</v>
+        <v>-2.19</v>
       </c>
     </row>
     <row r="175">
       <c r="A175" s="1" t="inlineStr">
         <is>
-          <t>SID/BBD</t>
+          <t>SGML/ASAI</t>
         </is>
       </c>
       <c r="B175" s="21" t="inlineStr">
         <is>
-          <t>SID</t>
+          <t>SGML</t>
         </is>
       </c>
       <c r="C175" t="n">
-        <v>2.46</v>
+        <v>-2.59</v>
       </c>
     </row>
     <row r="176">
       <c r="A176" s="1" t="inlineStr">
         <is>
-          <t>SID/BSBR</t>
+          <t>SGML/CSAN</t>
         </is>
       </c>
       <c r="B176" s="21" t="inlineStr">
         <is>
-          <t>SID</t>
+          <t>SGML</t>
         </is>
       </c>
       <c r="C176" t="n">
-        <v>2.01</v>
+        <v>-2.42</v>
       </c>
     </row>
     <row r="177">
       <c r="A177" s="1" t="inlineStr">
         <is>
-          <t>SID/GOL</t>
+          <t>SGML/PBR</t>
         </is>
       </c>
       <c r="B177" s="21" t="inlineStr">
         <is>
-          <t>SID</t>
+          <t>SGML</t>
         </is>
       </c>
       <c r="C177" t="n">
-        <v>4.17</v>
+        <v>-2.15</v>
       </c>
     </row>
     <row r="178">
       <c r="A178" s="1" t="inlineStr">
         <is>
-          <t>SID/GGB</t>
+          <t>SGML/BBD</t>
         </is>
       </c>
       <c r="B178" s="21" t="inlineStr">
         <is>
-          <t>SID</t>
+          <t>SGML</t>
         </is>
       </c>
       <c r="C178" t="n">
-        <v>2.32</v>
+        <v>-2.27</v>
       </c>
     </row>
     <row r="179">
       <c r="A179" s="1" t="inlineStr">
         <is>
-          <t>SID/VALE</t>
+          <t>SGML/BSBR</t>
         </is>
       </c>
       <c r="B179" s="21" t="inlineStr">
         <is>
-          <t>SID</t>
+          <t>SGML</t>
         </is>
       </c>
       <c r="C179" t="n">
-        <v>2.83</v>
+        <v>-2.61</v>
       </c>
     </row>
     <row r="180">
       <c r="A180" s="1" t="inlineStr">
         <is>
-          <t>SID/SGML</t>
+          <t>SGML/ITUB</t>
         </is>
       </c>
       <c r="B180" s="21" t="inlineStr">
         <is>
-          <t>SID</t>
+          <t>SGML</t>
         </is>
       </c>
       <c r="C180" t="n">
-        <v>4.09</v>
+        <v>-2.44</v>
       </c>
     </row>
     <row r="181">
       <c r="A181" s="1" t="inlineStr">
         <is>
-          <t>GGB/ITUB</t>
-        </is>
-      </c>
-      <c r="B181" s="22" t="inlineStr">
-        <is>
-          <t>GGB</t>
+          <t>SGML/PAGS</t>
+        </is>
+      </c>
+      <c r="B181" s="21" t="inlineStr">
+        <is>
+          <t>SGML</t>
         </is>
       </c>
       <c r="C181" t="n">
-        <v>-2.02</v>
+        <v>-2.68</v>
       </c>
     </row>
     <row r="182">
       <c r="A182" s="1" t="inlineStr">
         <is>
-          <t>GGB/PAGS</t>
-        </is>
-      </c>
-      <c r="B182" s="22" t="inlineStr">
-        <is>
-          <t>GGB</t>
+          <t>SGML/STNE</t>
+        </is>
+      </c>
+      <c r="B182" s="21" t="inlineStr">
+        <is>
+          <t>SGML</t>
         </is>
       </c>
       <c r="C182" t="n">
@@ -3373,1081 +3349,796 @@
     <row r="183">
       <c r="A183" s="1" t="inlineStr">
         <is>
-          <t>GGB/GOL</t>
-        </is>
-      </c>
-      <c r="B183" s="22" t="inlineStr">
-        <is>
-          <t>GGB</t>
+          <t>SGML/ERJ</t>
+        </is>
+      </c>
+      <c r="B183" s="21" t="inlineStr">
+        <is>
+          <t>SGML</t>
         </is>
       </c>
       <c r="C183" t="n">
-        <v>3.6</v>
+        <v>-2.53</v>
       </c>
     </row>
     <row r="184">
       <c r="A184" s="1" t="inlineStr">
         <is>
-          <t>GGB/SGML</t>
-        </is>
-      </c>
-      <c r="B184" s="22" t="inlineStr">
-        <is>
-          <t>GGB</t>
+          <t>SGML/SID</t>
+        </is>
+      </c>
+      <c r="B184" s="21" t="inlineStr">
+        <is>
+          <t>SGML</t>
         </is>
       </c>
       <c r="C184" t="n">
-        <v>3.88</v>
+        <v>-2.51</v>
       </c>
     </row>
     <row r="185">
       <c r="A185" s="1" t="inlineStr">
         <is>
-          <t>GGB/EBR</t>
-        </is>
-      </c>
-      <c r="B185" s="22" t="inlineStr">
-        <is>
-          <t>GGB</t>
+          <t>SGML/GGB</t>
+        </is>
+      </c>
+      <c r="B185" s="21" t="inlineStr">
+        <is>
+          <t>SGML</t>
         </is>
       </c>
       <c r="C185" t="n">
-        <v>-2.06</v>
+        <v>-2.97</v>
       </c>
     </row>
     <row r="186">
       <c r="A186" s="1" t="inlineStr">
         <is>
-          <t>SGML/VIV</t>
-        </is>
-      </c>
-      <c r="B186" s="23" t="inlineStr">
+          <t>SGML/SUZ</t>
+        </is>
+      </c>
+      <c r="B186" s="21" t="inlineStr">
         <is>
           <t>SGML</t>
         </is>
       </c>
       <c r="C186" t="n">
-        <v>-2.39</v>
+        <v>-2.18</v>
       </c>
     </row>
     <row r="187">
       <c r="A187" s="1" t="inlineStr">
         <is>
-          <t>SGML/TIMB</t>
-        </is>
-      </c>
-      <c r="B187" s="23" t="inlineStr">
+          <t>SGML/BAK</t>
+        </is>
+      </c>
+      <c r="B187" s="21" t="inlineStr">
         <is>
           <t>SGML</t>
         </is>
       </c>
       <c r="C187" t="n">
-        <v>-2.32</v>
+        <v>-3.01</v>
       </c>
     </row>
     <row r="188">
       <c r="A188" s="1" t="inlineStr">
         <is>
-          <t>SGML/ABEV</t>
-        </is>
-      </c>
-      <c r="B188" s="23" t="inlineStr">
+          <t>SGML/VALE</t>
+        </is>
+      </c>
+      <c r="B188" s="21" t="inlineStr">
         <is>
           <t>SGML</t>
         </is>
       </c>
       <c r="C188" t="n">
-        <v>-3.05</v>
+        <v>-2.53</v>
       </c>
     </row>
     <row r="189">
       <c r="A189" s="1" t="inlineStr">
         <is>
-          <t>SGML/NTCO</t>
-        </is>
-      </c>
-      <c r="B189" s="23" t="inlineStr">
+          <t>SGML/EBR</t>
+        </is>
+      </c>
+      <c r="B189" s="21" t="inlineStr">
         <is>
           <t>SGML</t>
         </is>
       </c>
       <c r="C189" t="n">
-        <v>-2.32</v>
+        <v>-2.52</v>
       </c>
     </row>
     <row r="190">
       <c r="A190" s="1" t="inlineStr">
         <is>
-          <t>SGML/ASAI</t>
-        </is>
-      </c>
-      <c r="B190" s="23" t="inlineStr">
+          <t>SGML/CIG</t>
+        </is>
+      </c>
+      <c r="B190" s="21" t="inlineStr">
         <is>
           <t>SGML</t>
         </is>
       </c>
       <c r="C190" t="n">
-        <v>-2.65</v>
+        <v>-2.69</v>
       </c>
     </row>
     <row r="191">
       <c r="A191" s="1" t="inlineStr">
         <is>
-          <t>SGML/CSAN</t>
-        </is>
-      </c>
-      <c r="B191" s="23" t="inlineStr">
+          <t>SGML/ELP</t>
+        </is>
+      </c>
+      <c r="B191" s="21" t="inlineStr">
         <is>
           <t>SGML</t>
         </is>
       </c>
       <c r="C191" t="n">
-        <v>-2.45</v>
+        <v>-2.14</v>
       </c>
     </row>
     <row r="192">
       <c r="A192" s="1" t="inlineStr">
         <is>
-          <t>SGML/PBR</t>
-        </is>
-      </c>
-      <c r="B192" s="23" t="inlineStr">
+          <t>SGML/SBS</t>
+        </is>
+      </c>
+      <c r="B192" s="21" t="inlineStr">
         <is>
           <t>SGML</t>
         </is>
       </c>
       <c r="C192" t="n">
-        <v>-2.18</v>
+        <v>-2.25</v>
       </c>
     </row>
     <row r="193">
       <c r="A193" s="1" t="inlineStr">
         <is>
-          <t>SGML/UGP</t>
-        </is>
-      </c>
-      <c r="B193" s="23" t="inlineStr">
-        <is>
-          <t>SGML</t>
+          <t>EBR/ABEV</t>
+        </is>
+      </c>
+      <c r="B193" s="22" t="inlineStr">
+        <is>
+          <t>EBR</t>
         </is>
       </c>
       <c r="C193" t="n">
-        <v>-2.01</v>
+        <v>2.41</v>
       </c>
     </row>
     <row r="194">
       <c r="A194" s="1" t="inlineStr">
         <is>
-          <t>SGML/BBD</t>
-        </is>
-      </c>
-      <c r="B194" s="23" t="inlineStr">
-        <is>
-          <t>SGML</t>
+          <t>EBR/BBD</t>
+        </is>
+      </c>
+      <c r="B194" s="22" t="inlineStr">
+        <is>
+          <t>EBR</t>
         </is>
       </c>
       <c r="C194" t="n">
-        <v>-2.34</v>
+        <v>4</v>
       </c>
     </row>
     <row r="195">
       <c r="A195" s="1" t="inlineStr">
         <is>
-          <t>SGML/BSBR</t>
-        </is>
-      </c>
-      <c r="B195" s="23" t="inlineStr">
-        <is>
-          <t>SGML</t>
+          <t>EBR/BSBR</t>
+        </is>
+      </c>
+      <c r="B195" s="22" t="inlineStr">
+        <is>
+          <t>EBR</t>
         </is>
       </c>
       <c r="C195" t="n">
-        <v>-2.65</v>
+        <v>2.37</v>
       </c>
     </row>
     <row r="196">
       <c r="A196" s="1" t="inlineStr">
         <is>
-          <t>SGML/ITUB</t>
-        </is>
-      </c>
-      <c r="B196" s="23" t="inlineStr">
-        <is>
-          <t>SGML</t>
+          <t>EBR/GOL</t>
+        </is>
+      </c>
+      <c r="B196" s="22" t="inlineStr">
+        <is>
+          <t>EBR</t>
         </is>
       </c>
       <c r="C196" t="n">
-        <v>-2.49</v>
+        <v>4.35</v>
       </c>
     </row>
     <row r="197">
       <c r="A197" s="1" t="inlineStr">
         <is>
-          <t>SGML/PAGS</t>
-        </is>
-      </c>
-      <c r="B197" s="23" t="inlineStr">
-        <is>
-          <t>SGML</t>
+          <t>EBR/GGB</t>
+        </is>
+      </c>
+      <c r="B197" s="22" t="inlineStr">
+        <is>
+          <t>EBR</t>
         </is>
       </c>
       <c r="C197" t="n">
-        <v>-2.8</v>
+        <v>2.16</v>
       </c>
     </row>
     <row r="198">
       <c r="A198" s="1" t="inlineStr">
         <is>
-          <t>SGML/STNE</t>
-        </is>
-      </c>
-      <c r="B198" s="23" t="inlineStr">
-        <is>
-          <t>SGML</t>
+          <t>EBR/SGML</t>
+        </is>
+      </c>
+      <c r="B198" s="22" t="inlineStr">
+        <is>
+          <t>EBR</t>
         </is>
       </c>
       <c r="C198" t="n">
-        <v>-2.27</v>
+        <v>3.7</v>
       </c>
     </row>
     <row r="199">
       <c r="A199" s="1" t="inlineStr">
         <is>
-          <t>SGML/ERJ</t>
+          <t>ELP/PBR</t>
         </is>
       </c>
       <c r="B199" s="23" t="inlineStr">
         <is>
-          <t>SGML</t>
+          <t>ELP</t>
         </is>
       </c>
       <c r="C199" t="n">
-        <v>-2.61</v>
+        <v>-2.31</v>
       </c>
     </row>
     <row r="200">
       <c r="A200" s="1" t="inlineStr">
         <is>
-          <t>SGML/SID</t>
+          <t>ELP/UGP</t>
         </is>
       </c>
       <c r="B200" s="23" t="inlineStr">
         <is>
-          <t>SGML</t>
+          <t>ELP</t>
         </is>
       </c>
       <c r="C200" t="n">
-        <v>-2.53</v>
+        <v>-2.2</v>
       </c>
     </row>
     <row r="201">
       <c r="A201" s="1" t="inlineStr">
         <is>
-          <t>SGML/GGB</t>
+          <t>ELP/ITUB</t>
         </is>
       </c>
       <c r="B201" s="23" t="inlineStr">
         <is>
-          <t>SGML</t>
+          <t>ELP</t>
         </is>
       </c>
       <c r="C201" t="n">
-        <v>-3.04</v>
+        <v>-2.21</v>
       </c>
     </row>
     <row r="202">
       <c r="A202" s="1" t="inlineStr">
         <is>
-          <t>SGML/SUZ</t>
+          <t>ELP/NU</t>
         </is>
       </c>
       <c r="B202" s="23" t="inlineStr">
         <is>
-          <t>SGML</t>
+          <t>ELP</t>
         </is>
       </c>
       <c r="C202" t="n">
-        <v>-2.2</v>
+        <v>-2.01</v>
       </c>
     </row>
     <row r="203">
       <c r="A203" s="1" t="inlineStr">
         <is>
-          <t>SGML/BAK</t>
+          <t>ELP/GOL</t>
         </is>
       </c>
       <c r="B203" s="23" t="inlineStr">
         <is>
-          <t>SGML</t>
+          <t>ELP</t>
         </is>
       </c>
       <c r="C203" t="n">
-        <v>-2.82</v>
+        <v>4.22</v>
       </c>
     </row>
     <row r="204">
       <c r="A204" s="1" t="inlineStr">
         <is>
-          <t>SGML/VALE</t>
+          <t>ELP/SGML</t>
         </is>
       </c>
       <c r="B204" s="23" t="inlineStr">
         <is>
-          <t>SGML</t>
+          <t>ELP</t>
         </is>
       </c>
       <c r="C204" t="n">
-        <v>-2.53</v>
+        <v>3.32</v>
       </c>
     </row>
     <row r="205">
       <c r="A205" s="1" t="inlineStr">
         <is>
-          <t>SGML/EBR</t>
+          <t>ELP/SBS</t>
         </is>
       </c>
       <c r="B205" s="23" t="inlineStr">
         <is>
-          <t>SGML</t>
+          <t>ELP</t>
         </is>
       </c>
       <c r="C205" t="n">
-        <v>-2.61</v>
+        <v>-2.46</v>
       </c>
     </row>
     <row r="206">
       <c r="A206" s="1" t="inlineStr">
         <is>
-          <t>SGML/CIG</t>
-        </is>
-      </c>
-      <c r="B206" s="23" t="inlineStr">
-        <is>
-          <t>SGML</t>
+          <t>SBS/VIV</t>
+        </is>
+      </c>
+      <c r="B206" s="24" t="inlineStr">
+        <is>
+          <t>SBS</t>
         </is>
       </c>
       <c r="C206" t="n">
-        <v>-2.72</v>
+        <v>2.43</v>
       </c>
     </row>
     <row r="207">
       <c r="A207" s="1" t="inlineStr">
         <is>
-          <t>SGML/ELP</t>
-        </is>
-      </c>
-      <c r="B207" s="23" t="inlineStr">
-        <is>
-          <t>SGML</t>
+          <t>SBS/TIMB</t>
+        </is>
+      </c>
+      <c r="B207" s="24" t="inlineStr">
+        <is>
+          <t>SBS</t>
         </is>
       </c>
       <c r="C207" t="n">
-        <v>-2.19</v>
+        <v>2.81</v>
       </c>
     </row>
     <row r="208">
       <c r="A208" s="1" t="inlineStr">
         <is>
-          <t>SGML/SBS</t>
-        </is>
-      </c>
-      <c r="B208" s="23" t="inlineStr">
-        <is>
-          <t>SGML</t>
+          <t>SBS/ABEV</t>
+        </is>
+      </c>
+      <c r="B208" s="24" t="inlineStr">
+        <is>
+          <t>SBS</t>
         </is>
       </c>
       <c r="C208" t="n">
-        <v>-2.29</v>
+        <v>2.56</v>
       </c>
     </row>
     <row r="209">
       <c r="A209" s="1" t="inlineStr">
         <is>
-          <t>EBR/ABEV</t>
+          <t>SBS/CSAN</t>
         </is>
       </c>
       <c r="B209" s="24" t="inlineStr">
         <is>
-          <t>EBR</t>
+          <t>SBS</t>
         </is>
       </c>
       <c r="C209" t="n">
-        <v>2.42</v>
+        <v>2.05</v>
       </c>
     </row>
     <row r="210">
       <c r="A210" s="1" t="inlineStr">
         <is>
-          <t>EBR/BBD</t>
+          <t>SBS/BBD</t>
         </is>
       </c>
       <c r="B210" s="24" t="inlineStr">
         <is>
-          <t>EBR</t>
+          <t>SBS</t>
         </is>
       </c>
       <c r="C210" t="n">
-        <v>4.36</v>
+        <v>3.53</v>
       </c>
     </row>
     <row r="211">
       <c r="A211" s="1" t="inlineStr">
         <is>
-          <t>EBR/BSBR</t>
+          <t>SBS/BSBR</t>
         </is>
       </c>
       <c r="B211" s="24" t="inlineStr">
         <is>
-          <t>EBR</t>
+          <t>SBS</t>
         </is>
       </c>
       <c r="C211" t="n">
-        <v>3.06</v>
+        <v>2.51</v>
       </c>
     </row>
     <row r="212">
       <c r="A212" s="1" t="inlineStr">
         <is>
-          <t>EBR/GOL</t>
+          <t>SBS/AZUL</t>
         </is>
       </c>
       <c r="B212" s="24" t="inlineStr">
         <is>
-          <t>EBR</t>
+          <t>SBS</t>
         </is>
       </c>
       <c r="C212" t="n">
-        <v>4.27</v>
+        <v>2.64</v>
       </c>
     </row>
     <row r="213">
       <c r="A213" s="1" t="inlineStr">
         <is>
-          <t>EBR/GGB</t>
+          <t>SBS/GOL</t>
         </is>
       </c>
       <c r="B213" s="24" t="inlineStr">
         <is>
-          <t>EBR</t>
+          <t>SBS</t>
         </is>
       </c>
       <c r="C213" t="n">
-        <v>2.45</v>
+        <v>4.41</v>
       </c>
     </row>
     <row r="214">
       <c r="A214" s="1" t="inlineStr">
         <is>
-          <t>EBR/BAK</t>
+          <t>SBS/GGB</t>
         </is>
       </c>
       <c r="B214" s="24" t="inlineStr">
         <is>
-          <t>EBR</t>
+          <t>SBS</t>
         </is>
       </c>
       <c r="C214" t="n">
-        <v>2.08</v>
+        <v>2.45</v>
       </c>
     </row>
     <row r="215">
       <c r="A215" s="1" t="inlineStr">
         <is>
-          <t>EBR/VALE</t>
+          <t>SBS/SUZ</t>
         </is>
       </c>
       <c r="B215" s="24" t="inlineStr">
         <is>
-          <t>EBR</t>
+          <t>SBS</t>
         </is>
       </c>
       <c r="C215" t="n">
-        <v>2.02</v>
+        <v>2.64</v>
       </c>
     </row>
     <row r="216">
       <c r="A216" s="1" t="inlineStr">
         <is>
-          <t>EBR/SGML</t>
+          <t>SBS/VALE</t>
         </is>
       </c>
       <c r="B216" s="24" t="inlineStr">
         <is>
-          <t>EBR</t>
+          <t>SBS</t>
         </is>
       </c>
       <c r="C216" t="n">
-        <v>4.01</v>
+        <v>2.36</v>
       </c>
     </row>
     <row r="217">
       <c r="A217" s="1" t="inlineStr">
         <is>
-          <t>ELP/VIV</t>
-        </is>
-      </c>
-      <c r="B217" s="25" t="inlineStr">
-        <is>
-          <t>ELP</t>
+          <t>SBS/SGML</t>
+        </is>
+      </c>
+      <c r="B217" s="24" t="inlineStr">
+        <is>
+          <t>SBS</t>
         </is>
       </c>
       <c r="C217" t="n">
-        <v>-2.19</v>
+        <v>3.79</v>
       </c>
     </row>
     <row r="218">
       <c r="A218" s="1" t="inlineStr">
         <is>
-          <t>ELP/TIMB</t>
-        </is>
-      </c>
-      <c r="B218" s="25" t="inlineStr">
-        <is>
-          <t>ELP</t>
+          <t>SBS/EBR</t>
+        </is>
+      </c>
+      <c r="B218" s="24" t="inlineStr">
+        <is>
+          <t>SBS</t>
         </is>
       </c>
       <c r="C218" t="n">
-        <v>-2.25</v>
+        <v>2.06</v>
       </c>
     </row>
     <row r="219">
       <c r="A219" s="1" t="inlineStr">
         <is>
-          <t>ELP/PBR</t>
-        </is>
-      </c>
-      <c r="B219" s="25" t="inlineStr">
-        <is>
-          <t>ELP</t>
+          <t>SBS/CIG</t>
+        </is>
+      </c>
+      <c r="B219" s="24" t="inlineStr">
+        <is>
+          <t>SBS</t>
         </is>
       </c>
       <c r="C219" t="n">
-        <v>-2.2</v>
+        <v>2.13</v>
       </c>
     </row>
     <row r="220">
       <c r="A220" s="1" t="inlineStr">
         <is>
-          <t>ELP/UGP</t>
-        </is>
-      </c>
-      <c r="B220" s="25" t="inlineStr">
-        <is>
-          <t>ELP</t>
+          <t>SBS/ELP</t>
+        </is>
+      </c>
+      <c r="B220" s="24" t="inlineStr">
+        <is>
+          <t>SBS</t>
         </is>
       </c>
       <c r="C220" t="n">
-        <v>-2.17</v>
+        <v>2.78</v>
       </c>
     </row>
     <row r="221">
       <c r="A221" s="1" t="inlineStr">
         <is>
-          <t>ELP/ITUB</t>
+          <t>BCH/SQM</t>
         </is>
       </c>
       <c r="B221" s="25" t="inlineStr">
         <is>
-          <t>ELP</t>
+          <t>BCH</t>
         </is>
       </c>
       <c r="C221" t="n">
-        <v>-2.1</v>
+        <v>2.44</v>
       </c>
     </row>
     <row r="222">
       <c r="A222" s="1" t="inlineStr">
         <is>
-          <t>ELP/NU</t>
-        </is>
-      </c>
-      <c r="B222" s="25" t="inlineStr">
-        <is>
-          <t>ELP</t>
+          <t>BSAC/CCU</t>
+        </is>
+      </c>
+      <c r="B222" s="26" t="inlineStr">
+        <is>
+          <t>BSAC</t>
         </is>
       </c>
       <c r="C222" t="n">
-        <v>-2.05</v>
+        <v>2.01</v>
       </c>
     </row>
     <row r="223">
       <c r="A223" s="1" t="inlineStr">
         <is>
-          <t>ELP/GOL</t>
-        </is>
-      </c>
-      <c r="B223" s="25" t="inlineStr">
-        <is>
-          <t>ELP</t>
+          <t>BSAC/SQM</t>
+        </is>
+      </c>
+      <c r="B223" s="26" t="inlineStr">
+        <is>
+          <t>BSAC</t>
         </is>
       </c>
       <c r="C223" t="n">
-        <v>4.06</v>
+        <v>2.55</v>
       </c>
     </row>
     <row r="224">
       <c r="A224" s="1" t="inlineStr">
         <is>
-          <t>ELP/SGML</t>
-        </is>
-      </c>
-      <c r="B224" s="25" t="inlineStr">
-        <is>
-          <t>ELP</t>
+          <t>EXTO/EC</t>
+        </is>
+      </c>
+      <c r="B224" s="27" t="inlineStr">
+        <is>
+          <t>EXTO</t>
         </is>
       </c>
       <c r="C224" t="n">
-        <v>3.54</v>
+        <v>-2.06</v>
       </c>
     </row>
     <row r="225">
       <c r="A225" s="1" t="inlineStr">
         <is>
-          <t>ELP/SBS</t>
-        </is>
-      </c>
-      <c r="B225" s="25" t="inlineStr">
-        <is>
-          <t>ELP</t>
+          <t>EXTO/CIB</t>
+        </is>
+      </c>
+      <c r="B225" s="27" t="inlineStr">
+        <is>
+          <t>EXTO</t>
         </is>
       </c>
       <c r="C225" t="n">
-        <v>-2.4</v>
+        <v>-2.46</v>
       </c>
     </row>
     <row r="226">
       <c r="A226" s="1" t="inlineStr">
         <is>
-          <t>SBS/ABEV</t>
-        </is>
-      </c>
-      <c r="B226" s="26" t="inlineStr">
-        <is>
-          <t>SBS</t>
+          <t>EC/EXTO</t>
+        </is>
+      </c>
+      <c r="B226" s="28" t="inlineStr">
+        <is>
+          <t>EC</t>
         </is>
       </c>
       <c r="C226" t="n">
-        <v>2.4</v>
+        <v>2.32</v>
       </c>
     </row>
     <row r="227">
       <c r="A227" s="1" t="inlineStr">
         <is>
-          <t>SBS/CSAN</t>
-        </is>
-      </c>
-      <c r="B227" s="26" t="inlineStr">
-        <is>
-          <t>SBS</t>
+          <t>CIB/EXTO</t>
+        </is>
+      </c>
+      <c r="B227" s="29" t="inlineStr">
+        <is>
+          <t>CIB</t>
         </is>
       </c>
       <c r="C227" t="n">
-        <v>2.11</v>
+        <v>3.17</v>
       </c>
     </row>
     <row r="228">
       <c r="A228" s="1" t="inlineStr">
         <is>
-          <t>SBS/BBD</t>
-        </is>
-      </c>
-      <c r="B228" s="26" t="inlineStr">
-        <is>
-          <t>SBS</t>
+          <t>TGLS/EXTO</t>
+        </is>
+      </c>
+      <c r="B228" s="30" t="inlineStr">
+        <is>
+          <t>TGLS</t>
         </is>
       </c>
       <c r="C228" t="n">
-        <v>3.5</v>
+        <v>2.5</v>
       </c>
     </row>
     <row r="229">
       <c r="A229" s="1" t="inlineStr">
         <is>
-          <t>SBS/BSBR</t>
-        </is>
-      </c>
-      <c r="B229" s="26" t="inlineStr">
-        <is>
-          <t>SBS</t>
+          <t>KOF/AMX</t>
+        </is>
+      </c>
+      <c r="B229" s="31" t="inlineStr">
+        <is>
+          <t>KOF</t>
         </is>
       </c>
       <c r="C229" t="n">
-        <v>2.62</v>
+        <v>2.18</v>
       </c>
     </row>
     <row r="230">
       <c r="A230" s="1" t="inlineStr">
         <is>
-          <t>SBS/AZUL</t>
-        </is>
-      </c>
-      <c r="B230" s="26" t="inlineStr">
-        <is>
-          <t>SBS</t>
+          <t>KOF/OMAB</t>
+        </is>
+      </c>
+      <c r="B230" s="31" t="inlineStr">
+        <is>
+          <t>KOF</t>
         </is>
       </c>
       <c r="C230" t="n">
-        <v>2.46</v>
+        <v>2.3</v>
       </c>
     </row>
     <row r="231">
       <c r="A231" s="1" t="inlineStr">
         <is>
-          <t>SBS/GOL</t>
-        </is>
-      </c>
-      <c r="B231" s="26" t="inlineStr">
-        <is>
-          <t>SBS</t>
+          <t>KOF/VTMX</t>
+        </is>
+      </c>
+      <c r="B231" s="31" t="inlineStr">
+        <is>
+          <t>KOF</t>
         </is>
       </c>
       <c r="C231" t="n">
-        <v>4.2</v>
+        <v>3.86</v>
       </c>
     </row>
     <row r="232">
       <c r="A232" s="1" t="inlineStr">
         <is>
-          <t>SBS/GGB</t>
-        </is>
-      </c>
-      <c r="B232" s="26" t="inlineStr">
-        <is>
-          <t>SBS</t>
+          <t>ASR/AMX</t>
+        </is>
+      </c>
+      <c r="B232" s="32" t="inlineStr">
+        <is>
+          <t>ASR</t>
         </is>
       </c>
       <c r="C232" t="n">
-        <v>2.52</v>
+        <v>2.23</v>
       </c>
     </row>
     <row r="233">
       <c r="A233" s="1" t="inlineStr">
         <is>
-          <t>SBS/SUZ</t>
-        </is>
-      </c>
-      <c r="B233" s="26" t="inlineStr">
-        <is>
-          <t>SBS</t>
+          <t>ASR/VLRS</t>
+        </is>
+      </c>
+      <c r="B233" s="32" t="inlineStr">
+        <is>
+          <t>ASR</t>
         </is>
       </c>
       <c r="C233" t="n">
-        <v>2.78</v>
+        <v>2.12</v>
       </c>
     </row>
     <row r="234">
       <c r="A234" s="1" t="inlineStr">
         <is>
-          <t>SBS/BAK</t>
-        </is>
-      </c>
-      <c r="B234" s="26" t="inlineStr">
-        <is>
-          <t>SBS</t>
+          <t>ASR/OMAB</t>
+        </is>
+      </c>
+      <c r="B234" s="32" t="inlineStr">
+        <is>
+          <t>ASR</t>
         </is>
       </c>
       <c r="C234" t="n">
-        <v>2.25</v>
+        <v>2.68</v>
       </c>
     </row>
     <row r="235">
       <c r="A235" s="1" t="inlineStr">
         <is>
-          <t>SBS/VALE</t>
-        </is>
-      </c>
-      <c r="B235" s="26" t="inlineStr">
-        <is>
-          <t>SBS</t>
+          <t>ASR/PAC</t>
+        </is>
+      </c>
+      <c r="B235" s="32" t="inlineStr">
+        <is>
+          <t>ASR</t>
         </is>
       </c>
       <c r="C235" t="n">
-        <v>2.54</v>
-      </c>
-    </row>
-    <row r="236">
-      <c r="A236" s="1" t="inlineStr">
-        <is>
-          <t>SBS/SGML</t>
-        </is>
-      </c>
-      <c r="B236" s="26" t="inlineStr">
-        <is>
-          <t>SBS</t>
-        </is>
-      </c>
-      <c r="C236" t="n">
-        <v>3.94</v>
-      </c>
-    </row>
-    <row r="237">
-      <c r="A237" s="1" t="inlineStr">
-        <is>
-          <t>SBS/CIG</t>
-        </is>
-      </c>
-      <c r="B237" s="26" t="inlineStr">
-        <is>
-          <t>SBS</t>
-        </is>
-      </c>
-      <c r="C237" t="n">
-        <v>2.21</v>
-      </c>
-    </row>
-    <row r="238">
-      <c r="A238" s="1" t="inlineStr">
-        <is>
-          <t>SBS/ELP</t>
-        </is>
-      </c>
-      <c r="B238" s="26" t="inlineStr">
-        <is>
-          <t>SBS</t>
-        </is>
-      </c>
-      <c r="C238" t="n">
-        <v>2.67</v>
-      </c>
-    </row>
-    <row r="239">
-      <c r="A239" s="1" t="inlineStr">
-        <is>
-          <t>CCU/SQM</t>
-        </is>
-      </c>
-      <c r="B239" s="27" t="inlineStr">
-        <is>
-          <t>CCU</t>
-        </is>
-      </c>
-      <c r="C239" t="n">
-        <v>2.37</v>
-      </c>
-    </row>
-    <row r="240">
-      <c r="A240" s="1" t="inlineStr">
-        <is>
-          <t>BCH/SQM</t>
-        </is>
-      </c>
-      <c r="B240" s="28" t="inlineStr">
-        <is>
-          <t>BCH</t>
-        </is>
-      </c>
-      <c r="C240" t="n">
-        <v>2.64</v>
-      </c>
-    </row>
-    <row r="241">
-      <c r="A241" s="1" t="inlineStr">
-        <is>
-          <t>BSAC/SQM</t>
-        </is>
-      </c>
-      <c r="B241" s="29" t="inlineStr">
-        <is>
-          <t>BSAC</t>
-        </is>
-      </c>
-      <c r="C241" t="n">
-        <v>2.72</v>
-      </c>
-    </row>
-    <row r="242">
-      <c r="A242" s="1" t="inlineStr">
-        <is>
-          <t>SQM/CCU</t>
-        </is>
-      </c>
-      <c r="B242" s="30" t="inlineStr">
-        <is>
-          <t>SQM</t>
-        </is>
-      </c>
-      <c r="C242" t="n">
-        <v>-2.02</v>
-      </c>
-    </row>
-    <row r="243">
-      <c r="A243" s="1" t="inlineStr">
-        <is>
-          <t>EXTO/EC</t>
-        </is>
-      </c>
-      <c r="B243" s="31" t="inlineStr">
-        <is>
-          <t>EXTO</t>
-        </is>
-      </c>
-      <c r="C243" t="n">
-        <v>-2.11</v>
-      </c>
-    </row>
-    <row r="244">
-      <c r="A244" s="1" t="inlineStr">
-        <is>
-          <t>EXTO/CIB</t>
-        </is>
-      </c>
-      <c r="B244" s="31" t="inlineStr">
-        <is>
-          <t>EXTO</t>
-        </is>
-      </c>
-      <c r="C244" t="n">
-        <v>-2.52</v>
-      </c>
-    </row>
-    <row r="245">
-      <c r="A245" s="1" t="inlineStr">
-        <is>
-          <t>EC/EXTO</t>
-        </is>
-      </c>
-      <c r="B245" s="32" t="inlineStr">
-        <is>
-          <t>EC</t>
-        </is>
-      </c>
-      <c r="C245" t="n">
-        <v>2.39</v>
-      </c>
-    </row>
-    <row r="246">
-      <c r="A246" s="1" t="inlineStr">
-        <is>
-          <t>CIB/EXTO</t>
-        </is>
-      </c>
-      <c r="B246" s="33" t="inlineStr">
-        <is>
-          <t>CIB</t>
-        </is>
-      </c>
-      <c r="C246" t="n">
-        <v>3.29</v>
-      </c>
-    </row>
-    <row r="247">
-      <c r="A247" s="1" t="inlineStr">
-        <is>
-          <t>TGLS/EXTO</t>
-        </is>
-      </c>
-      <c r="B247" s="34" t="inlineStr">
-        <is>
-          <t>TGLS</t>
-        </is>
-      </c>
-      <c r="C247" t="n">
-        <v>2.51</v>
-      </c>
-    </row>
-    <row r="248">
-      <c r="A248" s="1" t="inlineStr">
-        <is>
-          <t>KOF/AMX</t>
-        </is>
-      </c>
-      <c r="B248" s="35" t="inlineStr">
-        <is>
-          <t>KOF</t>
-        </is>
-      </c>
-      <c r="C248" t="n">
-        <v>2.35</v>
-      </c>
-    </row>
-    <row r="249">
-      <c r="A249" s="1" t="inlineStr">
-        <is>
-          <t>KOF/OMAB</t>
-        </is>
-      </c>
-      <c r="B249" s="35" t="inlineStr">
-        <is>
-          <t>KOF</t>
-        </is>
-      </c>
-      <c r="C249" t="n">
-        <v>2.17</v>
-      </c>
-    </row>
-    <row r="250">
-      <c r="A250" s="1" t="inlineStr">
-        <is>
-          <t>KOF/VTMX</t>
-        </is>
-      </c>
-      <c r="B250" s="35" t="inlineStr">
-        <is>
-          <t>KOF</t>
-        </is>
-      </c>
-      <c r="C250" t="n">
-        <v>3.26</v>
-      </c>
-    </row>
-    <row r="251">
-      <c r="A251" s="1" t="inlineStr">
-        <is>
-          <t>ASR/AMX</t>
-        </is>
-      </c>
-      <c r="B251" s="36" t="inlineStr">
-        <is>
-          <t>ASR</t>
-        </is>
-      </c>
-      <c r="C251" t="n">
-        <v>2.36</v>
-      </c>
-    </row>
-    <row r="252">
-      <c r="A252" s="1" t="inlineStr">
-        <is>
-          <t>ASR/VLRS</t>
-        </is>
-      </c>
-      <c r="B252" s="36" t="inlineStr">
-        <is>
-          <t>ASR</t>
-        </is>
-      </c>
-      <c r="C252" t="n">
-        <v>2.21</v>
-      </c>
-    </row>
-    <row r="253">
-      <c r="A253" s="1" t="inlineStr">
-        <is>
-          <t>ASR/OMAB</t>
-        </is>
-      </c>
-      <c r="B253" s="36" t="inlineStr">
-        <is>
-          <t>ASR</t>
-        </is>
-      </c>
-      <c r="C253" t="n">
-        <v>2.41</v>
-      </c>
-    </row>
-    <row r="254">
-      <c r="A254" s="1" t="inlineStr">
-        <is>
-          <t>ASR/PAC</t>
-        </is>
-      </c>
-      <c r="B254" s="36" t="inlineStr">
-        <is>
-          <t>ASR</t>
-        </is>
-      </c>
-      <c r="C254" t="n">
-        <v>2.65</v>
+        <v>2.88</v>
       </c>
     </row>
   </sheetData>

</xml_diff>